<commit_message>
Added optional '--batch' arg to 'rnn.py' and made it so batch files now use this arg to call 'rnn' and have it correctly reference external files.
</commit_message>
<xml_diff>
--- a/documentation/model_shapes.xlsx
+++ b/documentation/model_shapes.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D337"/>
+  <dimension ref="A1:D345"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7108,6 +7108,166 @@
         <v>60</v>
       </c>
     </row>
+    <row r="338">
+      <c r="A338" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B338" t="inlineStr">
+        <is>
+          <t>sensorMagneticField</t>
+        </is>
+      </c>
+      <c r="C338" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D338" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="339">
+      <c r="A339" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B339" t="inlineStr">
+        <is>
+          <t>sensorMagneticField</t>
+        </is>
+      </c>
+      <c r="C339" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D339" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="340">
+      <c r="A340" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B340" t="inlineStr">
+        <is>
+          <t>jointAngle</t>
+        </is>
+      </c>
+      <c r="C340" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D340" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="341">
+      <c r="A341" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B341" t="inlineStr">
+        <is>
+          <t>AD</t>
+        </is>
+      </c>
+      <c r="C341" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D341" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="342">
+      <c r="A342" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B342" t="inlineStr">
+        <is>
+          <t>sensorMagneticField</t>
+        </is>
+      </c>
+      <c r="C342" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D342" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="343">
+      <c r="A343" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B343" t="inlineStr">
+        <is>
+          <t>sensorMagneticField</t>
+        </is>
+      </c>
+      <c r="C343" t="inlineStr">
+        <is>
+          <t>overall</t>
+        </is>
+      </c>
+      <c r="D343" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="344">
+      <c r="A344" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B344" t="inlineStr">
+        <is>
+          <t>sensorMagneticField</t>
+        </is>
+      </c>
+      <c r="C344" t="inlineStr">
+        <is>
+          <t>acts</t>
+        </is>
+      </c>
+      <c r="D344" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="345">
+      <c r="A345" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B345" t="inlineStr">
+        <is>
+          <t>jointAngle</t>
+        </is>
+      </c>
+      <c r="C345" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D345" t="n">
+        <v>60</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>

<commit_message>
Added more to the experiments and results discussion, added batch scripts to run the model prediction sets, added to the relevant README for these scripts and modified the script ecosystem overview as such, started a system setup description, and added a document on system choices made.
</commit_message>
<xml_diff>
--- a/documentation/model_shapes.xlsx
+++ b/documentation/model_shapes.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D345"/>
+  <dimension ref="A1:D452"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7268,6 +7268,2146 @@
         <v>60</v>
       </c>
     </row>
+    <row r="346">
+      <c r="A346" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B346" t="inlineStr">
+        <is>
+          <t>jointAngle</t>
+        </is>
+      </c>
+      <c r="C346" t="inlineStr">
+        <is>
+          <t>overall</t>
+        </is>
+      </c>
+      <c r="D346" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="347">
+      <c r="A347" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B347" t="inlineStr">
+        <is>
+          <t>jointAngle</t>
+        </is>
+      </c>
+      <c r="C347" t="inlineStr">
+        <is>
+          <t>acts</t>
+        </is>
+      </c>
+      <c r="D347" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="348">
+      <c r="A348" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B348" t="inlineStr">
+        <is>
+          <t>AD</t>
+        </is>
+      </c>
+      <c r="C348" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D348" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="349">
+      <c r="A349" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B349" t="inlineStr">
+        <is>
+          <t>AD</t>
+        </is>
+      </c>
+      <c r="C349" t="inlineStr">
+        <is>
+          <t>overall</t>
+        </is>
+      </c>
+      <c r="D349" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="350">
+      <c r="A350" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B350" t="inlineStr">
+        <is>
+          <t>AD</t>
+        </is>
+      </c>
+      <c r="C350" t="inlineStr">
+        <is>
+          <t>acts</t>
+        </is>
+      </c>
+      <c r="D350" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="351">
+      <c r="A351" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B351" t="inlineStr">
+        <is>
+          <t>position</t>
+        </is>
+      </c>
+      <c r="C351" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D351" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="352">
+      <c r="A352" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B352" t="inlineStr">
+        <is>
+          <t>position</t>
+        </is>
+      </c>
+      <c r="C352" t="inlineStr">
+        <is>
+          <t>overall</t>
+        </is>
+      </c>
+      <c r="D352" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="353">
+      <c r="A353" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B353" t="inlineStr">
+        <is>
+          <t>position</t>
+        </is>
+      </c>
+      <c r="C353" t="inlineStr">
+        <is>
+          <t>acts</t>
+        </is>
+      </c>
+      <c r="D353" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="354">
+      <c r="A354" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B354" t="inlineStr">
+        <is>
+          <t>sensorMagneticField</t>
+        </is>
+      </c>
+      <c r="C354" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D354" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="355">
+      <c r="A355" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B355" t="inlineStr">
+        <is>
+          <t>sensorMagneticField</t>
+        </is>
+      </c>
+      <c r="C355" t="inlineStr">
+        <is>
+          <t>overall</t>
+        </is>
+      </c>
+      <c r="D355" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="356">
+      <c r="A356" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B356" t="inlineStr">
+        <is>
+          <t>sensorMagneticField</t>
+        </is>
+      </c>
+      <c r="C356" t="inlineStr">
+        <is>
+          <t>acts</t>
+        </is>
+      </c>
+      <c r="D356" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="357">
+      <c r="A357" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B357" t="inlineStr">
+        <is>
+          <t>jointAngle</t>
+        </is>
+      </c>
+      <c r="C357" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D357" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="358">
+      <c r="A358" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B358" t="inlineStr">
+        <is>
+          <t>jointAngle</t>
+        </is>
+      </c>
+      <c r="C358" t="inlineStr">
+        <is>
+          <t>overall</t>
+        </is>
+      </c>
+      <c r="D358" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="359">
+      <c r="A359" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B359" t="inlineStr">
+        <is>
+          <t>jointAngle</t>
+        </is>
+      </c>
+      <c r="C359" t="inlineStr">
+        <is>
+          <t>acts</t>
+        </is>
+      </c>
+      <c r="D359" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="360">
+      <c r="A360" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B360" t="inlineStr">
+        <is>
+          <t>AD</t>
+        </is>
+      </c>
+      <c r="C360" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D360" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="361">
+      <c r="A361" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B361" t="inlineStr">
+        <is>
+          <t>AD</t>
+        </is>
+      </c>
+      <c r="C361" t="inlineStr">
+        <is>
+          <t>overall</t>
+        </is>
+      </c>
+      <c r="D361" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="362">
+      <c r="A362" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B362" t="inlineStr">
+        <is>
+          <t>AD</t>
+        </is>
+      </c>
+      <c r="C362" t="inlineStr">
+        <is>
+          <t>acts</t>
+        </is>
+      </c>
+      <c r="D362" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="363">
+      <c r="A363" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B363" t="inlineStr">
+        <is>
+          <t>AD</t>
+        </is>
+      </c>
+      <c r="C363" t="inlineStr">
+        <is>
+          <t>acts</t>
+        </is>
+      </c>
+      <c r="D363" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="364">
+      <c r="A364" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B364" t="inlineStr">
+        <is>
+          <t>AD</t>
+        </is>
+      </c>
+      <c r="C364" t="inlineStr">
+        <is>
+          <t>acts</t>
+        </is>
+      </c>
+      <c r="D364" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="365">
+      <c r="A365" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B365" t="inlineStr">
+        <is>
+          <t>AD</t>
+        </is>
+      </c>
+      <c r="C365" t="inlineStr">
+        <is>
+          <t>acts</t>
+        </is>
+      </c>
+      <c r="D365" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="366">
+      <c r="A366" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B366" t="inlineStr">
+        <is>
+          <t>AD</t>
+        </is>
+      </c>
+      <c r="C366" t="inlineStr">
+        <is>
+          <t>acts</t>
+        </is>
+      </c>
+      <c r="D366" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="367">
+      <c r="A367" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B367" t="inlineStr">
+        <is>
+          <t>AD</t>
+        </is>
+      </c>
+      <c r="C367" t="inlineStr">
+        <is>
+          <t>acts</t>
+        </is>
+      </c>
+      <c r="D367" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="368">
+      <c r="A368" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B368" t="inlineStr">
+        <is>
+          <t>AD</t>
+        </is>
+      </c>
+      <c r="C368" t="inlineStr">
+        <is>
+          <t>acts</t>
+        </is>
+      </c>
+      <c r="D368" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="369">
+      <c r="A369" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B369" t="inlineStr">
+        <is>
+          <t>AD</t>
+        </is>
+      </c>
+      <c r="C369" t="inlineStr">
+        <is>
+          <t>acts</t>
+        </is>
+      </c>
+      <c r="D369" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="370">
+      <c r="A370" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B370" t="inlineStr">
+        <is>
+          <t>AD</t>
+        </is>
+      </c>
+      <c r="C370" t="inlineStr">
+        <is>
+          <t>acts</t>
+        </is>
+      </c>
+      <c r="D370" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="371">
+      <c r="A371" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B371" t="inlineStr">
+        <is>
+          <t>AD</t>
+        </is>
+      </c>
+      <c r="C371" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D371" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="372">
+      <c r="A372" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B372" t="inlineStr">
+        <is>
+          <t>AD</t>
+        </is>
+      </c>
+      <c r="C372" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D372" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="373">
+      <c r="A373" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B373" t="inlineStr">
+        <is>
+          <t>AD</t>
+        </is>
+      </c>
+      <c r="C373" t="inlineStr">
+        <is>
+          <t>overall</t>
+        </is>
+      </c>
+      <c r="D373" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="374">
+      <c r="A374" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B374" t="inlineStr">
+        <is>
+          <t>AD</t>
+        </is>
+      </c>
+      <c r="C374" t="inlineStr">
+        <is>
+          <t>acts</t>
+        </is>
+      </c>
+      <c r="D374" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="375">
+      <c r="A375" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B375" t="inlineStr">
+        <is>
+          <t>AD</t>
+        </is>
+      </c>
+      <c r="C375" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D375" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="376">
+      <c r="A376" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B376" t="inlineStr">
+        <is>
+          <t>AD</t>
+        </is>
+      </c>
+      <c r="C376" t="inlineStr">
+        <is>
+          <t>overall</t>
+        </is>
+      </c>
+      <c r="D376" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="377">
+      <c r="A377" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B377" t="inlineStr">
+        <is>
+          <t>AD</t>
+        </is>
+      </c>
+      <c r="C377" t="inlineStr">
+        <is>
+          <t>acts</t>
+        </is>
+      </c>
+      <c r="D377" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="378">
+      <c r="A378" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B378" t="inlineStr">
+        <is>
+          <t>AD</t>
+        </is>
+      </c>
+      <c r="C378" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D378" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="379">
+      <c r="A379" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B379" t="inlineStr">
+        <is>
+          <t>AD</t>
+        </is>
+      </c>
+      <c r="C379" t="inlineStr">
+        <is>
+          <t>overall</t>
+        </is>
+      </c>
+      <c r="D379" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="380">
+      <c r="A380" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B380" t="inlineStr">
+        <is>
+          <t>AD</t>
+        </is>
+      </c>
+      <c r="C380" t="inlineStr">
+        <is>
+          <t>acts</t>
+        </is>
+      </c>
+      <c r="D380" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="381">
+      <c r="A381" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B381" t="inlineStr">
+        <is>
+          <t>AD</t>
+        </is>
+      </c>
+      <c r="C381" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D381" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="382">
+      <c r="A382" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B382" t="inlineStr">
+        <is>
+          <t>AD</t>
+        </is>
+      </c>
+      <c r="C382" t="inlineStr">
+        <is>
+          <t>overall</t>
+        </is>
+      </c>
+      <c r="D382" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="383">
+      <c r="A383" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B383" t="inlineStr">
+        <is>
+          <t>AD</t>
+        </is>
+      </c>
+      <c r="C383" t="inlineStr">
+        <is>
+          <t>acts</t>
+        </is>
+      </c>
+      <c r="D383" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="384">
+      <c r="A384" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B384" t="inlineStr">
+        <is>
+          <t>AD</t>
+        </is>
+      </c>
+      <c r="C384" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D384" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="385">
+      <c r="A385" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B385" t="inlineStr">
+        <is>
+          <t>AD</t>
+        </is>
+      </c>
+      <c r="C385" t="inlineStr">
+        <is>
+          <t>overall</t>
+        </is>
+      </c>
+      <c r="D385" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="386">
+      <c r="A386" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B386" t="inlineStr">
+        <is>
+          <t>AD</t>
+        </is>
+      </c>
+      <c r="C386" t="inlineStr">
+        <is>
+          <t>acts</t>
+        </is>
+      </c>
+      <c r="D386" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="387">
+      <c r="A387" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B387" t="inlineStr">
+        <is>
+          <t>position</t>
+        </is>
+      </c>
+      <c r="C387" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D387" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="388">
+      <c r="A388" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B388" t="inlineStr">
+        <is>
+          <t>sensorMagneticField</t>
+        </is>
+      </c>
+      <c r="C388" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D388" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="389">
+      <c r="A389" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B389" t="inlineStr">
+        <is>
+          <t>jointAngle</t>
+        </is>
+      </c>
+      <c r="C389" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D389" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="390">
+      <c r="A390" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B390" t="inlineStr">
+        <is>
+          <t>position</t>
+        </is>
+      </c>
+      <c r="C390" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D390" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="391">
+      <c r="A391" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B391" t="inlineStr">
+        <is>
+          <t>sensorMagneticField</t>
+        </is>
+      </c>
+      <c r="C391" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D391" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="392">
+      <c r="A392" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B392" t="inlineStr">
+        <is>
+          <t>jointAngle</t>
+        </is>
+      </c>
+      <c r="C392" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D392" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="393">
+      <c r="A393" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B393" t="inlineStr">
+        <is>
+          <t>position</t>
+        </is>
+      </c>
+      <c r="C393" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D393" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="394">
+      <c r="A394" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B394" t="inlineStr">
+        <is>
+          <t>position</t>
+        </is>
+      </c>
+      <c r="C394" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D394" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="395">
+      <c r="A395" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B395" t="inlineStr">
+        <is>
+          <t>position</t>
+        </is>
+      </c>
+      <c r="C395" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D395" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="396">
+      <c r="A396" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B396" t="inlineStr">
+        <is>
+          <t>position</t>
+        </is>
+      </c>
+      <c r="C396" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D396" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="397">
+      <c r="A397" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B397" t="inlineStr">
+        <is>
+          <t>position</t>
+        </is>
+      </c>
+      <c r="C397" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D397" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="398">
+      <c r="A398" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B398" t="inlineStr">
+        <is>
+          <t>position</t>
+        </is>
+      </c>
+      <c r="C398" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D398" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="399">
+      <c r="A399" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B399" t="inlineStr">
+        <is>
+          <t>position</t>
+        </is>
+      </c>
+      <c r="C399" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D399" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="400">
+      <c r="A400" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B400" t="inlineStr">
+        <is>
+          <t>sensorMagneticField</t>
+        </is>
+      </c>
+      <c r="C400" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D400" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="401">
+      <c r="A401" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B401" t="inlineStr">
+        <is>
+          <t>position</t>
+        </is>
+      </c>
+      <c r="C401" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D401" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="402">
+      <c r="A402" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B402" t="inlineStr">
+        <is>
+          <t>sensorMagneticField</t>
+        </is>
+      </c>
+      <c r="C402" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D402" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="403">
+      <c r="A403" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B403" t="inlineStr">
+        <is>
+          <t>position</t>
+        </is>
+      </c>
+      <c r="C403" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D403" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="404">
+      <c r="A404" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B404" t="inlineStr">
+        <is>
+          <t>sensorMagneticField</t>
+        </is>
+      </c>
+      <c r="C404" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D404" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="405">
+      <c r="A405" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B405" t="inlineStr">
+        <is>
+          <t>position</t>
+        </is>
+      </c>
+      <c r="C405" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D405" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="406">
+      <c r="A406" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B406" t="inlineStr">
+        <is>
+          <t>sensorMagneticField</t>
+        </is>
+      </c>
+      <c r="C406" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D406" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="407">
+      <c r="A407" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B407" t="inlineStr">
+        <is>
+          <t>AD</t>
+        </is>
+      </c>
+      <c r="C407" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D407" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="408">
+      <c r="A408" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B408" t="inlineStr">
+        <is>
+          <t>position</t>
+        </is>
+      </c>
+      <c r="C408" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D408" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="409">
+      <c r="A409" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B409" t="inlineStr">
+        <is>
+          <t>sensorMagneticField</t>
+        </is>
+      </c>
+      <c r="C409" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D409" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="410">
+      <c r="A410" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B410" t="inlineStr">
+        <is>
+          <t>position</t>
+        </is>
+      </c>
+      <c r="C410" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D410" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="411">
+      <c r="A411" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B411" t="inlineStr">
+        <is>
+          <t>sensorMagneticField</t>
+        </is>
+      </c>
+      <c r="C411" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D411" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="412">
+      <c r="A412" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B412" t="inlineStr">
+        <is>
+          <t>jointAngle</t>
+        </is>
+      </c>
+      <c r="C412" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D412" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="413">
+      <c r="A413" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B413" t="inlineStr">
+        <is>
+          <t>position</t>
+        </is>
+      </c>
+      <c r="C413" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D413" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="414">
+      <c r="A414" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B414" t="inlineStr">
+        <is>
+          <t>sensorMagneticField</t>
+        </is>
+      </c>
+      <c r="C414" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D414" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="415">
+      <c r="A415" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B415" t="inlineStr">
+        <is>
+          <t>jointAngle</t>
+        </is>
+      </c>
+      <c r="C415" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D415" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="416">
+      <c r="A416" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B416" t="inlineStr">
+        <is>
+          <t>position</t>
+        </is>
+      </c>
+      <c r="C416" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D416" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="417">
+      <c r="A417" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B417" t="inlineStr">
+        <is>
+          <t>position</t>
+        </is>
+      </c>
+      <c r="C417" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D417" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="418">
+      <c r="A418" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B418" t="inlineStr">
+        <is>
+          <t>sensorMagneticField</t>
+        </is>
+      </c>
+      <c r="C418" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D418" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="419">
+      <c r="A419" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B419" t="inlineStr">
+        <is>
+          <t>jointAngle</t>
+        </is>
+      </c>
+      <c r="C419" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D419" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="420">
+      <c r="A420" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B420" t="inlineStr">
+        <is>
+          <t>position</t>
+        </is>
+      </c>
+      <c r="C420" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D420" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="421">
+      <c r="A421" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B421" t="inlineStr">
+        <is>
+          <t>sensorMagneticField</t>
+        </is>
+      </c>
+      <c r="C421" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D421" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="422">
+      <c r="A422" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B422" t="inlineStr">
+        <is>
+          <t>jointAngle</t>
+        </is>
+      </c>
+      <c r="C422" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D422" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="423">
+      <c r="A423" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B423" t="inlineStr">
+        <is>
+          <t>position</t>
+        </is>
+      </c>
+      <c r="C423" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D423" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="424">
+      <c r="A424" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B424" t="inlineStr">
+        <is>
+          <t>sensorMagneticField</t>
+        </is>
+      </c>
+      <c r="C424" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D424" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="425">
+      <c r="A425" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B425" t="inlineStr">
+        <is>
+          <t>position</t>
+        </is>
+      </c>
+      <c r="C425" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D425" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="426">
+      <c r="A426" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B426" t="inlineStr">
+        <is>
+          <t>sensorMagneticField</t>
+        </is>
+      </c>
+      <c r="C426" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D426" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="427">
+      <c r="A427" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B427" t="inlineStr">
+        <is>
+          <t>jointAngle</t>
+        </is>
+      </c>
+      <c r="C427" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D427" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="428">
+      <c r="A428" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B428" t="inlineStr">
+        <is>
+          <t>position</t>
+        </is>
+      </c>
+      <c r="C428" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D428" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="429">
+      <c r="A429" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B429" t="inlineStr">
+        <is>
+          <t>sensorMagneticField</t>
+        </is>
+      </c>
+      <c r="C429" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D429" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="430">
+      <c r="A430" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B430" t="inlineStr">
+        <is>
+          <t>jointAngle</t>
+        </is>
+      </c>
+      <c r="C430" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D430" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="431">
+      <c r="A431" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B431" t="inlineStr">
+        <is>
+          <t>position</t>
+        </is>
+      </c>
+      <c r="C431" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D431" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="432">
+      <c r="A432" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B432" t="inlineStr">
+        <is>
+          <t>position</t>
+        </is>
+      </c>
+      <c r="C432" t="inlineStr">
+        <is>
+          <t>overall</t>
+        </is>
+      </c>
+      <c r="D432" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="433">
+      <c r="A433" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B433" t="inlineStr">
+        <is>
+          <t>position</t>
+        </is>
+      </c>
+      <c r="C433" t="inlineStr">
+        <is>
+          <t>acts</t>
+        </is>
+      </c>
+      <c r="D433" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="434">
+      <c r="A434" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B434" t="inlineStr">
+        <is>
+          <t>sensorMagneticField</t>
+        </is>
+      </c>
+      <c r="C434" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D434" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="435">
+      <c r="A435" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B435" t="inlineStr">
+        <is>
+          <t>sensorMagneticField</t>
+        </is>
+      </c>
+      <c r="C435" t="inlineStr">
+        <is>
+          <t>overall</t>
+        </is>
+      </c>
+      <c r="D435" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="436">
+      <c r="A436" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B436" t="inlineStr">
+        <is>
+          <t>sensorMagneticField</t>
+        </is>
+      </c>
+      <c r="C436" t="inlineStr">
+        <is>
+          <t>acts</t>
+        </is>
+      </c>
+      <c r="D436" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="437">
+      <c r="A437" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B437" t="inlineStr">
+        <is>
+          <t>jointAngle</t>
+        </is>
+      </c>
+      <c r="C437" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D437" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="438">
+      <c r="A438" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B438" t="inlineStr">
+        <is>
+          <t>jointAngle</t>
+        </is>
+      </c>
+      <c r="C438" t="inlineStr">
+        <is>
+          <t>overall</t>
+        </is>
+      </c>
+      <c r="D438" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="439">
+      <c r="A439" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B439" t="inlineStr">
+        <is>
+          <t>jointAngle</t>
+        </is>
+      </c>
+      <c r="C439" t="inlineStr">
+        <is>
+          <t>acts</t>
+        </is>
+      </c>
+      <c r="D439" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="440">
+      <c r="A440" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B440" t="inlineStr">
+        <is>
+          <t>AD</t>
+        </is>
+      </c>
+      <c r="C440" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D440" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="441">
+      <c r="A441" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B441" t="inlineStr">
+        <is>
+          <t>AD</t>
+        </is>
+      </c>
+      <c r="C441" t="inlineStr">
+        <is>
+          <t>overall</t>
+        </is>
+      </c>
+      <c r="D441" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="442">
+      <c r="A442" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B442" t="inlineStr">
+        <is>
+          <t>AD</t>
+        </is>
+      </c>
+      <c r="C442" t="inlineStr">
+        <is>
+          <t>acts</t>
+        </is>
+      </c>
+      <c r="D442" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="443">
+      <c r="A443" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B443" t="inlineStr">
+        <is>
+          <t>position</t>
+        </is>
+      </c>
+      <c r="C443" t="inlineStr">
+        <is>
+          <t>acts</t>
+        </is>
+      </c>
+      <c r="D443" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="444">
+      <c r="A444" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B444" t="inlineStr">
+        <is>
+          <t>sensorMagneticField</t>
+        </is>
+      </c>
+      <c r="C444" t="inlineStr">
+        <is>
+          <t>acts</t>
+        </is>
+      </c>
+      <c r="D444" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="445">
+      <c r="A445" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B445" t="inlineStr">
+        <is>
+          <t>jointAngle</t>
+        </is>
+      </c>
+      <c r="C445" t="inlineStr">
+        <is>
+          <t>acts</t>
+        </is>
+      </c>
+      <c r="D445" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="446">
+      <c r="A446" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B446" t="inlineStr">
+        <is>
+          <t>AD</t>
+        </is>
+      </c>
+      <c r="C446" t="inlineStr">
+        <is>
+          <t>acts</t>
+        </is>
+      </c>
+      <c r="D446" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="447">
+      <c r="A447" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B447" t="inlineStr">
+        <is>
+          <t>AD</t>
+        </is>
+      </c>
+      <c r="C447" t="inlineStr">
+        <is>
+          <t>acts</t>
+        </is>
+      </c>
+      <c r="D447" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="448">
+      <c r="A448" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B448" t="inlineStr">
+        <is>
+          <t>AD</t>
+        </is>
+      </c>
+      <c r="C448" t="inlineStr">
+        <is>
+          <t>acts</t>
+        </is>
+      </c>
+      <c r="D448" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="449">
+      <c r="A449" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B449" t="inlineStr">
+        <is>
+          <t>AD</t>
+        </is>
+      </c>
+      <c r="C449" t="inlineStr">
+        <is>
+          <t>acts</t>
+        </is>
+      </c>
+      <c r="D449" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="450">
+      <c r="A450" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B450" t="inlineStr">
+        <is>
+          <t>AD</t>
+        </is>
+      </c>
+      <c r="C450" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D450" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="451">
+      <c r="A451" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B451" t="inlineStr">
+        <is>
+          <t>AD</t>
+        </is>
+      </c>
+      <c r="C451" t="inlineStr">
+        <is>
+          <t>overall</t>
+        </is>
+      </c>
+      <c r="D451" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="452">
+      <c r="A452" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B452" t="inlineStr">
+        <is>
+          <t>AD</t>
+        </is>
+      </c>
+      <c r="C452" t="inlineStr">
+        <is>
+          <t>acts</t>
+        </is>
+      </c>
+      <c r="D452" t="n">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>

<commit_message>
Carried out model prediction sets 12-16, modified the 'source' Python files and batch scripts to carry these out, and added a project overview, glossary of acronyms and terms, and an explanation of the reference documents used.
</commit_message>
<xml_diff>
--- a/documentation/model_shapes.xlsx
+++ b/documentation/model_shapes.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D994"/>
+  <dimension ref="A1:D1166"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -20248,6 +20248,3446 @@
         <v>10</v>
       </c>
     </row>
+    <row r="995">
+      <c r="A995" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B995" t="inlineStr">
+        <is>
+          <t>position</t>
+        </is>
+      </c>
+      <c r="C995" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D995" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="996">
+      <c r="A996" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B996" t="inlineStr">
+        <is>
+          <t>jointAngle</t>
+        </is>
+      </c>
+      <c r="C996" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D996" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="997">
+      <c r="A997" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B997" t="inlineStr">
+        <is>
+          <t>position</t>
+        </is>
+      </c>
+      <c r="C997" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D997" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="998">
+      <c r="A998" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B998" t="inlineStr">
+        <is>
+          <t>position</t>
+        </is>
+      </c>
+      <c r="C998" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D998" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="999">
+      <c r="A999" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B999" t="inlineStr">
+        <is>
+          <t>position</t>
+        </is>
+      </c>
+      <c r="C999" t="inlineStr">
+        <is>
+          <t>overall</t>
+        </is>
+      </c>
+      <c r="D999" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1000">
+      <c r="A1000" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1000" t="inlineStr">
+        <is>
+          <t>position</t>
+        </is>
+      </c>
+      <c r="C1000" t="inlineStr">
+        <is>
+          <t>acts</t>
+        </is>
+      </c>
+      <c r="D1000" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1001">
+      <c r="A1001" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1001" t="inlineStr">
+        <is>
+          <t>sensorMagneticField</t>
+        </is>
+      </c>
+      <c r="C1001" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D1001" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1002">
+      <c r="A1002" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1002" t="inlineStr">
+        <is>
+          <t>sensorMagneticField</t>
+        </is>
+      </c>
+      <c r="C1002" t="inlineStr">
+        <is>
+          <t>overall</t>
+        </is>
+      </c>
+      <c r="D1002" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1003">
+      <c r="A1003" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1003" t="inlineStr">
+        <is>
+          <t>sensorMagneticField</t>
+        </is>
+      </c>
+      <c r="C1003" t="inlineStr">
+        <is>
+          <t>acts</t>
+        </is>
+      </c>
+      <c r="D1003" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1004">
+      <c r="A1004" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1004" t="inlineStr">
+        <is>
+          <t>jointAngle</t>
+        </is>
+      </c>
+      <c r="C1004" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D1004" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1005">
+      <c r="A1005" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1005" t="inlineStr">
+        <is>
+          <t>jointAngle</t>
+        </is>
+      </c>
+      <c r="C1005" t="inlineStr">
+        <is>
+          <t>overall</t>
+        </is>
+      </c>
+      <c r="D1005" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1006">
+      <c r="A1006" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1006" t="inlineStr">
+        <is>
+          <t>jointAngle</t>
+        </is>
+      </c>
+      <c r="C1006" t="inlineStr">
+        <is>
+          <t>acts</t>
+        </is>
+      </c>
+      <c r="D1006" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1007">
+      <c r="A1007" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1007" t="inlineStr">
+        <is>
+          <t>AD</t>
+        </is>
+      </c>
+      <c r="C1007" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D1007" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="1008">
+      <c r="A1008" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1008" t="inlineStr">
+        <is>
+          <t>AD</t>
+        </is>
+      </c>
+      <c r="C1008" t="inlineStr">
+        <is>
+          <t>overall</t>
+        </is>
+      </c>
+      <c r="D1008" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="1009">
+      <c r="A1009" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1009" t="inlineStr">
+        <is>
+          <t>AD</t>
+        </is>
+      </c>
+      <c r="C1009" t="inlineStr">
+        <is>
+          <t>acts</t>
+        </is>
+      </c>
+      <c r="D1009" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="1010">
+      <c r="A1010" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1010" t="inlineStr">
+        <is>
+          <t>position</t>
+        </is>
+      </c>
+      <c r="C1010" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D1010" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1011">
+      <c r="A1011" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1011" t="inlineStr">
+        <is>
+          <t>position</t>
+        </is>
+      </c>
+      <c r="C1011" t="inlineStr">
+        <is>
+          <t>overall</t>
+        </is>
+      </c>
+      <c r="D1011" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1012">
+      <c r="A1012" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1012" t="inlineStr">
+        <is>
+          <t>position</t>
+        </is>
+      </c>
+      <c r="C1012" t="inlineStr">
+        <is>
+          <t>acts</t>
+        </is>
+      </c>
+      <c r="D1012" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1013">
+      <c r="A1013" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1013" t="inlineStr">
+        <is>
+          <t>sensorMagneticField</t>
+        </is>
+      </c>
+      <c r="C1013" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D1013" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1014">
+      <c r="A1014" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1014" t="inlineStr">
+        <is>
+          <t>sensorMagneticField</t>
+        </is>
+      </c>
+      <c r="C1014" t="inlineStr">
+        <is>
+          <t>overall</t>
+        </is>
+      </c>
+      <c r="D1014" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1015">
+      <c r="A1015" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1015" t="inlineStr">
+        <is>
+          <t>sensorMagneticField</t>
+        </is>
+      </c>
+      <c r="C1015" t="inlineStr">
+        <is>
+          <t>acts</t>
+        </is>
+      </c>
+      <c r="D1015" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1016">
+      <c r="A1016" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1016" t="inlineStr">
+        <is>
+          <t>jointAngle</t>
+        </is>
+      </c>
+      <c r="C1016" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D1016" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1017">
+      <c r="A1017" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1017" t="inlineStr">
+        <is>
+          <t>jointAngle</t>
+        </is>
+      </c>
+      <c r="C1017" t="inlineStr">
+        <is>
+          <t>overall</t>
+        </is>
+      </c>
+      <c r="D1017" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1018">
+      <c r="A1018" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1018" t="inlineStr">
+        <is>
+          <t>jointAngle</t>
+        </is>
+      </c>
+      <c r="C1018" t="inlineStr">
+        <is>
+          <t>acts</t>
+        </is>
+      </c>
+      <c r="D1018" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1019">
+      <c r="A1019" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1019" t="inlineStr">
+        <is>
+          <t>AD</t>
+        </is>
+      </c>
+      <c r="C1019" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D1019" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="1020">
+      <c r="A1020" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1020" t="inlineStr">
+        <is>
+          <t>AD</t>
+        </is>
+      </c>
+      <c r="C1020" t="inlineStr">
+        <is>
+          <t>overall</t>
+        </is>
+      </c>
+      <c r="D1020" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="1021">
+      <c r="A1021" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1021" t="inlineStr">
+        <is>
+          <t>AD</t>
+        </is>
+      </c>
+      <c r="C1021" t="inlineStr">
+        <is>
+          <t>acts</t>
+        </is>
+      </c>
+      <c r="D1021" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="1022">
+      <c r="A1022" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1022" t="inlineStr">
+        <is>
+          <t>position</t>
+        </is>
+      </c>
+      <c r="C1022" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D1022" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1023">
+      <c r="A1023" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1023" t="inlineStr">
+        <is>
+          <t>position</t>
+        </is>
+      </c>
+      <c r="C1023" t="inlineStr">
+        <is>
+          <t>overall</t>
+        </is>
+      </c>
+      <c r="D1023" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1024">
+      <c r="A1024" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1024" t="inlineStr">
+        <is>
+          <t>position</t>
+        </is>
+      </c>
+      <c r="C1024" t="inlineStr">
+        <is>
+          <t>acts</t>
+        </is>
+      </c>
+      <c r="D1024" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1025">
+      <c r="A1025" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1025" t="inlineStr">
+        <is>
+          <t>sensorMagneticField</t>
+        </is>
+      </c>
+      <c r="C1025" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D1025" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1026">
+      <c r="A1026" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1026" t="inlineStr">
+        <is>
+          <t>sensorMagneticField</t>
+        </is>
+      </c>
+      <c r="C1026" t="inlineStr">
+        <is>
+          <t>overall</t>
+        </is>
+      </c>
+      <c r="D1026" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1027">
+      <c r="A1027" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1027" t="inlineStr">
+        <is>
+          <t>sensorMagneticField</t>
+        </is>
+      </c>
+      <c r="C1027" t="inlineStr">
+        <is>
+          <t>acts</t>
+        </is>
+      </c>
+      <c r="D1027" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1028">
+      <c r="A1028" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1028" t="inlineStr">
+        <is>
+          <t>jointAngle</t>
+        </is>
+      </c>
+      <c r="C1028" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D1028" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1029">
+      <c r="A1029" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1029" t="inlineStr">
+        <is>
+          <t>jointAngle</t>
+        </is>
+      </c>
+      <c r="C1029" t="inlineStr">
+        <is>
+          <t>overall</t>
+        </is>
+      </c>
+      <c r="D1029" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1030">
+      <c r="A1030" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1030" t="inlineStr">
+        <is>
+          <t>jointAngle</t>
+        </is>
+      </c>
+      <c r="C1030" t="inlineStr">
+        <is>
+          <t>acts</t>
+        </is>
+      </c>
+      <c r="D1030" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1031">
+      <c r="A1031" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1031" t="inlineStr">
+        <is>
+          <t>AD</t>
+        </is>
+      </c>
+      <c r="C1031" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D1031" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="1032">
+      <c r="A1032" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1032" t="inlineStr">
+        <is>
+          <t>AD</t>
+        </is>
+      </c>
+      <c r="C1032" t="inlineStr">
+        <is>
+          <t>overall</t>
+        </is>
+      </c>
+      <c r="D1032" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="1033">
+      <c r="A1033" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1033" t="inlineStr">
+        <is>
+          <t>AD</t>
+        </is>
+      </c>
+      <c r="C1033" t="inlineStr">
+        <is>
+          <t>acts</t>
+        </is>
+      </c>
+      <c r="D1033" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="1034">
+      <c r="A1034" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1034" t="inlineStr">
+        <is>
+          <t>position</t>
+        </is>
+      </c>
+      <c r="C1034" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D1034" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1035">
+      <c r="A1035" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1035" t="inlineStr">
+        <is>
+          <t>position</t>
+        </is>
+      </c>
+      <c r="C1035" t="inlineStr">
+        <is>
+          <t>overall</t>
+        </is>
+      </c>
+      <c r="D1035" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1036">
+      <c r="A1036" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1036" t="inlineStr">
+        <is>
+          <t>position</t>
+        </is>
+      </c>
+      <c r="C1036" t="inlineStr">
+        <is>
+          <t>acts</t>
+        </is>
+      </c>
+      <c r="D1036" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1037">
+      <c r="A1037" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1037" t="inlineStr">
+        <is>
+          <t>sensorMagneticField</t>
+        </is>
+      </c>
+      <c r="C1037" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D1037" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1038">
+      <c r="A1038" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1038" t="inlineStr">
+        <is>
+          <t>sensorMagneticField</t>
+        </is>
+      </c>
+      <c r="C1038" t="inlineStr">
+        <is>
+          <t>overall</t>
+        </is>
+      </c>
+      <c r="D1038" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1039">
+      <c r="A1039" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1039" t="inlineStr">
+        <is>
+          <t>sensorMagneticField</t>
+        </is>
+      </c>
+      <c r="C1039" t="inlineStr">
+        <is>
+          <t>acts</t>
+        </is>
+      </c>
+      <c r="D1039" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1040">
+      <c r="A1040" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1040" t="inlineStr">
+        <is>
+          <t>jointAngle</t>
+        </is>
+      </c>
+      <c r="C1040" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D1040" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1041">
+      <c r="A1041" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1041" t="inlineStr">
+        <is>
+          <t>jointAngle</t>
+        </is>
+      </c>
+      <c r="C1041" t="inlineStr">
+        <is>
+          <t>overall</t>
+        </is>
+      </c>
+      <c r="D1041" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1042">
+      <c r="A1042" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1042" t="inlineStr">
+        <is>
+          <t>jointAngle</t>
+        </is>
+      </c>
+      <c r="C1042" t="inlineStr">
+        <is>
+          <t>acts</t>
+        </is>
+      </c>
+      <c r="D1042" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1043">
+      <c r="A1043" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1043" t="inlineStr">
+        <is>
+          <t>AD</t>
+        </is>
+      </c>
+      <c r="C1043" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D1043" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="1044">
+      <c r="A1044" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1044" t="inlineStr">
+        <is>
+          <t>AD</t>
+        </is>
+      </c>
+      <c r="C1044" t="inlineStr">
+        <is>
+          <t>overall</t>
+        </is>
+      </c>
+      <c r="D1044" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="1045">
+      <c r="A1045" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1045" t="inlineStr">
+        <is>
+          <t>AD</t>
+        </is>
+      </c>
+      <c r="C1045" t="inlineStr">
+        <is>
+          <t>acts</t>
+        </is>
+      </c>
+      <c r="D1045" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="1046">
+      <c r="A1046" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1046" t="inlineStr">
+        <is>
+          <t>position</t>
+        </is>
+      </c>
+      <c r="C1046" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D1046" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1047">
+      <c r="A1047" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1047" t="inlineStr">
+        <is>
+          <t>position</t>
+        </is>
+      </c>
+      <c r="C1047" t="inlineStr">
+        <is>
+          <t>overall</t>
+        </is>
+      </c>
+      <c r="D1047" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1048">
+      <c r="A1048" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1048" t="inlineStr">
+        <is>
+          <t>position</t>
+        </is>
+      </c>
+      <c r="C1048" t="inlineStr">
+        <is>
+          <t>acts</t>
+        </is>
+      </c>
+      <c r="D1048" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1049">
+      <c r="A1049" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1049" t="inlineStr">
+        <is>
+          <t>sensorMagneticField</t>
+        </is>
+      </c>
+      <c r="C1049" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D1049" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1050">
+      <c r="A1050" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1050" t="inlineStr">
+        <is>
+          <t>sensorMagneticField</t>
+        </is>
+      </c>
+      <c r="C1050" t="inlineStr">
+        <is>
+          <t>overall</t>
+        </is>
+      </c>
+      <c r="D1050" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1051">
+      <c r="A1051" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1051" t="inlineStr">
+        <is>
+          <t>sensorMagneticField</t>
+        </is>
+      </c>
+      <c r="C1051" t="inlineStr">
+        <is>
+          <t>acts</t>
+        </is>
+      </c>
+      <c r="D1051" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1052">
+      <c r="A1052" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1052" t="inlineStr">
+        <is>
+          <t>jointAngle</t>
+        </is>
+      </c>
+      <c r="C1052" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D1052" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1053">
+      <c r="A1053" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1053" t="inlineStr">
+        <is>
+          <t>jointAngle</t>
+        </is>
+      </c>
+      <c r="C1053" t="inlineStr">
+        <is>
+          <t>overall</t>
+        </is>
+      </c>
+      <c r="D1053" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1054">
+      <c r="A1054" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1054" t="inlineStr">
+        <is>
+          <t>jointAngle</t>
+        </is>
+      </c>
+      <c r="C1054" t="inlineStr">
+        <is>
+          <t>acts</t>
+        </is>
+      </c>
+      <c r="D1054" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1055">
+      <c r="A1055" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1055" t="inlineStr">
+        <is>
+          <t>AD</t>
+        </is>
+      </c>
+      <c r="C1055" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D1055" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="1056">
+      <c r="A1056" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1056" t="inlineStr">
+        <is>
+          <t>AD</t>
+        </is>
+      </c>
+      <c r="C1056" t="inlineStr">
+        <is>
+          <t>overall</t>
+        </is>
+      </c>
+      <c r="D1056" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="1057">
+      <c r="A1057" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1057" t="inlineStr">
+        <is>
+          <t>AD</t>
+        </is>
+      </c>
+      <c r="C1057" t="inlineStr">
+        <is>
+          <t>acts</t>
+        </is>
+      </c>
+      <c r="D1057" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="1058">
+      <c r="A1058" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1058" t="inlineStr">
+        <is>
+          <t>position</t>
+        </is>
+      </c>
+      <c r="C1058" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D1058" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1059">
+      <c r="A1059" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1059" t="inlineStr">
+        <is>
+          <t>position</t>
+        </is>
+      </c>
+      <c r="C1059" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D1059" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1060">
+      <c r="A1060" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1060" t="inlineStr">
+        <is>
+          <t>position</t>
+        </is>
+      </c>
+      <c r="C1060" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D1060" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1061">
+      <c r="A1061" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1061" t="inlineStr">
+        <is>
+          <t>position</t>
+        </is>
+      </c>
+      <c r="C1061" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D1061" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1062">
+      <c r="A1062" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1062" t="inlineStr">
+        <is>
+          <t>position</t>
+        </is>
+      </c>
+      <c r="C1062" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D1062" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1063">
+      <c r="A1063" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1063" t="inlineStr">
+        <is>
+          <t>position</t>
+        </is>
+      </c>
+      <c r="C1063" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D1063" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1064">
+      <c r="A1064" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1064" t="inlineStr">
+        <is>
+          <t>position</t>
+        </is>
+      </c>
+      <c r="C1064" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D1064" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1065">
+      <c r="A1065" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1065" t="inlineStr">
+        <is>
+          <t>position</t>
+        </is>
+      </c>
+      <c r="C1065" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D1065" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1066">
+      <c r="A1066" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1066" t="inlineStr">
+        <is>
+          <t>position</t>
+        </is>
+      </c>
+      <c r="C1066" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D1066" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1067">
+      <c r="A1067" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1067" t="inlineStr">
+        <is>
+          <t>position</t>
+        </is>
+      </c>
+      <c r="C1067" t="inlineStr">
+        <is>
+          <t>overall</t>
+        </is>
+      </c>
+      <c r="D1067" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1068">
+      <c r="A1068" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1068" t="inlineStr">
+        <is>
+          <t>position</t>
+        </is>
+      </c>
+      <c r="C1068" t="inlineStr">
+        <is>
+          <t>acts</t>
+        </is>
+      </c>
+      <c r="D1068" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1069">
+      <c r="A1069" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1069" t="inlineStr">
+        <is>
+          <t>position</t>
+        </is>
+      </c>
+      <c r="C1069" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D1069" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1070">
+      <c r="A1070" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1070" t="inlineStr">
+        <is>
+          <t>position</t>
+        </is>
+      </c>
+      <c r="C1070" t="inlineStr">
+        <is>
+          <t>overall</t>
+        </is>
+      </c>
+      <c r="D1070" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1071">
+      <c r="A1071" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1071" t="inlineStr">
+        <is>
+          <t>position</t>
+        </is>
+      </c>
+      <c r="C1071" t="inlineStr">
+        <is>
+          <t>acts</t>
+        </is>
+      </c>
+      <c r="D1071" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1072">
+      <c r="A1072" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1072" t="inlineStr">
+        <is>
+          <t>sensorMagneticField</t>
+        </is>
+      </c>
+      <c r="C1072" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D1072" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1073">
+      <c r="A1073" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1073" t="inlineStr">
+        <is>
+          <t>sensorMagneticField</t>
+        </is>
+      </c>
+      <c r="C1073" t="inlineStr">
+        <is>
+          <t>overall</t>
+        </is>
+      </c>
+      <c r="D1073" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1074">
+      <c r="A1074" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1074" t="inlineStr">
+        <is>
+          <t>sensorMagneticField</t>
+        </is>
+      </c>
+      <c r="C1074" t="inlineStr">
+        <is>
+          <t>acts</t>
+        </is>
+      </c>
+      <c r="D1074" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1075">
+      <c r="A1075" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1075" t="inlineStr">
+        <is>
+          <t>jointAngle</t>
+        </is>
+      </c>
+      <c r="C1075" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D1075" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1076">
+      <c r="A1076" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1076" t="inlineStr">
+        <is>
+          <t>jointAngle</t>
+        </is>
+      </c>
+      <c r="C1076" t="inlineStr">
+        <is>
+          <t>overall</t>
+        </is>
+      </c>
+      <c r="D1076" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1077">
+      <c r="A1077" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1077" t="inlineStr">
+        <is>
+          <t>jointAngle</t>
+        </is>
+      </c>
+      <c r="C1077" t="inlineStr">
+        <is>
+          <t>acts</t>
+        </is>
+      </c>
+      <c r="D1077" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1078">
+      <c r="A1078" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1078" t="inlineStr">
+        <is>
+          <t>AD</t>
+        </is>
+      </c>
+      <c r="C1078" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D1078" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="1079">
+      <c r="A1079" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1079" t="inlineStr">
+        <is>
+          <t>AD</t>
+        </is>
+      </c>
+      <c r="C1079" t="inlineStr">
+        <is>
+          <t>overall</t>
+        </is>
+      </c>
+      <c r="D1079" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="1080">
+      <c r="A1080" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1080" t="inlineStr">
+        <is>
+          <t>AD</t>
+        </is>
+      </c>
+      <c r="C1080" t="inlineStr">
+        <is>
+          <t>acts</t>
+        </is>
+      </c>
+      <c r="D1080" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="1081">
+      <c r="A1081" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1081" t="inlineStr">
+        <is>
+          <t>position</t>
+        </is>
+      </c>
+      <c r="C1081" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D1081" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1082">
+      <c r="A1082" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1082" t="inlineStr">
+        <is>
+          <t>position</t>
+        </is>
+      </c>
+      <c r="C1082" t="inlineStr">
+        <is>
+          <t>overall</t>
+        </is>
+      </c>
+      <c r="D1082" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1083">
+      <c r="A1083" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1083" t="inlineStr">
+        <is>
+          <t>position</t>
+        </is>
+      </c>
+      <c r="C1083" t="inlineStr">
+        <is>
+          <t>acts</t>
+        </is>
+      </c>
+      <c r="D1083" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1084">
+      <c r="A1084" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1084" t="inlineStr">
+        <is>
+          <t>sensorMagneticField</t>
+        </is>
+      </c>
+      <c r="C1084" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D1084" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1085">
+      <c r="A1085" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1085" t="inlineStr">
+        <is>
+          <t>sensorMagneticField</t>
+        </is>
+      </c>
+      <c r="C1085" t="inlineStr">
+        <is>
+          <t>overall</t>
+        </is>
+      </c>
+      <c r="D1085" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1086">
+      <c r="A1086" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1086" t="inlineStr">
+        <is>
+          <t>sensorMagneticField</t>
+        </is>
+      </c>
+      <c r="C1086" t="inlineStr">
+        <is>
+          <t>acts</t>
+        </is>
+      </c>
+      <c r="D1086" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1087">
+      <c r="A1087" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1087" t="inlineStr">
+        <is>
+          <t>jointAngle</t>
+        </is>
+      </c>
+      <c r="C1087" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D1087" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1088">
+      <c r="A1088" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1088" t="inlineStr">
+        <is>
+          <t>jointAngle</t>
+        </is>
+      </c>
+      <c r="C1088" t="inlineStr">
+        <is>
+          <t>overall</t>
+        </is>
+      </c>
+      <c r="D1088" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1089">
+      <c r="A1089" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1089" t="inlineStr">
+        <is>
+          <t>jointAngle</t>
+        </is>
+      </c>
+      <c r="C1089" t="inlineStr">
+        <is>
+          <t>acts</t>
+        </is>
+      </c>
+      <c r="D1089" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1090">
+      <c r="A1090" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1090" t="inlineStr">
+        <is>
+          <t>AD</t>
+        </is>
+      </c>
+      <c r="C1090" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D1090" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="1091">
+      <c r="A1091" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1091" t="inlineStr">
+        <is>
+          <t>AD</t>
+        </is>
+      </c>
+      <c r="C1091" t="inlineStr">
+        <is>
+          <t>overall</t>
+        </is>
+      </c>
+      <c r="D1091" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="1092">
+      <c r="A1092" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1092" t="inlineStr">
+        <is>
+          <t>AD</t>
+        </is>
+      </c>
+      <c r="C1092" t="inlineStr">
+        <is>
+          <t>acts</t>
+        </is>
+      </c>
+      <c r="D1092" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="1093">
+      <c r="A1093" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1093" t="inlineStr">
+        <is>
+          <t>position</t>
+        </is>
+      </c>
+      <c r="C1093" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D1093" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1094">
+      <c r="A1094" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1094" t="inlineStr">
+        <is>
+          <t>position</t>
+        </is>
+      </c>
+      <c r="C1094" t="inlineStr">
+        <is>
+          <t>overall</t>
+        </is>
+      </c>
+      <c r="D1094" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1095">
+      <c r="A1095" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1095" t="inlineStr">
+        <is>
+          <t>position</t>
+        </is>
+      </c>
+      <c r="C1095" t="inlineStr">
+        <is>
+          <t>acts</t>
+        </is>
+      </c>
+      <c r="D1095" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1096">
+      <c r="A1096" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1096" t="inlineStr">
+        <is>
+          <t>sensorMagneticField</t>
+        </is>
+      </c>
+      <c r="C1096" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D1096" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1097">
+      <c r="A1097" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1097" t="inlineStr">
+        <is>
+          <t>sensorMagneticField</t>
+        </is>
+      </c>
+      <c r="C1097" t="inlineStr">
+        <is>
+          <t>overall</t>
+        </is>
+      </c>
+      <c r="D1097" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1098">
+      <c r="A1098" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1098" t="inlineStr">
+        <is>
+          <t>sensorMagneticField</t>
+        </is>
+      </c>
+      <c r="C1098" t="inlineStr">
+        <is>
+          <t>acts</t>
+        </is>
+      </c>
+      <c r="D1098" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1099">
+      <c r="A1099" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1099" t="inlineStr">
+        <is>
+          <t>jointAngle</t>
+        </is>
+      </c>
+      <c r="C1099" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D1099" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1100">
+      <c r="A1100" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1100" t="inlineStr">
+        <is>
+          <t>jointAngle</t>
+        </is>
+      </c>
+      <c r="C1100" t="inlineStr">
+        <is>
+          <t>overall</t>
+        </is>
+      </c>
+      <c r="D1100" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1101">
+      <c r="A1101" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1101" t="inlineStr">
+        <is>
+          <t>jointAngle</t>
+        </is>
+      </c>
+      <c r="C1101" t="inlineStr">
+        <is>
+          <t>acts</t>
+        </is>
+      </c>
+      <c r="D1101" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1102">
+      <c r="A1102" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1102" t="inlineStr">
+        <is>
+          <t>AD</t>
+        </is>
+      </c>
+      <c r="C1102" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D1102" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="1103">
+      <c r="A1103" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1103" t="inlineStr">
+        <is>
+          <t>AD</t>
+        </is>
+      </c>
+      <c r="C1103" t="inlineStr">
+        <is>
+          <t>overall</t>
+        </is>
+      </c>
+      <c r="D1103" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="1104">
+      <c r="A1104" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1104" t="inlineStr">
+        <is>
+          <t>AD</t>
+        </is>
+      </c>
+      <c r="C1104" t="inlineStr">
+        <is>
+          <t>acts</t>
+        </is>
+      </c>
+      <c r="D1104" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="1105">
+      <c r="A1105" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1105" t="inlineStr">
+        <is>
+          <t>position</t>
+        </is>
+      </c>
+      <c r="C1105" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D1105" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1106">
+      <c r="A1106" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1106" t="inlineStr">
+        <is>
+          <t>position</t>
+        </is>
+      </c>
+      <c r="C1106" t="inlineStr">
+        <is>
+          <t>overall</t>
+        </is>
+      </c>
+      <c r="D1106" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1107">
+      <c r="A1107" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1107" t="inlineStr">
+        <is>
+          <t>position</t>
+        </is>
+      </c>
+      <c r="C1107" t="inlineStr">
+        <is>
+          <t>acts</t>
+        </is>
+      </c>
+      <c r="D1107" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1108">
+      <c r="A1108" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1108" t="inlineStr">
+        <is>
+          <t>sensorMagneticField</t>
+        </is>
+      </c>
+      <c r="C1108" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D1108" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1109">
+      <c r="A1109" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1109" t="inlineStr">
+        <is>
+          <t>sensorMagneticField</t>
+        </is>
+      </c>
+      <c r="C1109" t="inlineStr">
+        <is>
+          <t>overall</t>
+        </is>
+      </c>
+      <c r="D1109" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1110">
+      <c r="A1110" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1110" t="inlineStr">
+        <is>
+          <t>sensorMagneticField</t>
+        </is>
+      </c>
+      <c r="C1110" t="inlineStr">
+        <is>
+          <t>acts</t>
+        </is>
+      </c>
+      <c r="D1110" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1111">
+      <c r="A1111" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1111" t="inlineStr">
+        <is>
+          <t>jointAngle</t>
+        </is>
+      </c>
+      <c r="C1111" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D1111" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1112">
+      <c r="A1112" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1112" t="inlineStr">
+        <is>
+          <t>jointAngle</t>
+        </is>
+      </c>
+      <c r="C1112" t="inlineStr">
+        <is>
+          <t>overall</t>
+        </is>
+      </c>
+      <c r="D1112" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1113">
+      <c r="A1113" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1113" t="inlineStr">
+        <is>
+          <t>jointAngle</t>
+        </is>
+      </c>
+      <c r="C1113" t="inlineStr">
+        <is>
+          <t>acts</t>
+        </is>
+      </c>
+      <c r="D1113" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1114">
+      <c r="A1114" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1114" t="inlineStr">
+        <is>
+          <t>AD</t>
+        </is>
+      </c>
+      <c r="C1114" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D1114" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="1115">
+      <c r="A1115" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1115" t="inlineStr">
+        <is>
+          <t>AD</t>
+        </is>
+      </c>
+      <c r="C1115" t="inlineStr">
+        <is>
+          <t>overall</t>
+        </is>
+      </c>
+      <c r="D1115" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="1116">
+      <c r="A1116" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1116" t="inlineStr">
+        <is>
+          <t>AD</t>
+        </is>
+      </c>
+      <c r="C1116" t="inlineStr">
+        <is>
+          <t>acts</t>
+        </is>
+      </c>
+      <c r="D1116" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="1117">
+      <c r="A1117" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1117" t="inlineStr">
+        <is>
+          <t>position</t>
+        </is>
+      </c>
+      <c r="C1117" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D1117" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1118">
+      <c r="A1118" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1118" t="inlineStr">
+        <is>
+          <t>position</t>
+        </is>
+      </c>
+      <c r="C1118" t="inlineStr">
+        <is>
+          <t>overall</t>
+        </is>
+      </c>
+      <c r="D1118" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1119">
+      <c r="A1119" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1119" t="inlineStr">
+        <is>
+          <t>position</t>
+        </is>
+      </c>
+      <c r="C1119" t="inlineStr">
+        <is>
+          <t>acts</t>
+        </is>
+      </c>
+      <c r="D1119" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1120">
+      <c r="A1120" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1120" t="inlineStr">
+        <is>
+          <t>sensorMagneticField</t>
+        </is>
+      </c>
+      <c r="C1120" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D1120" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1121">
+      <c r="A1121" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1121" t="inlineStr">
+        <is>
+          <t>sensorMagneticField</t>
+        </is>
+      </c>
+      <c r="C1121" t="inlineStr">
+        <is>
+          <t>overall</t>
+        </is>
+      </c>
+      <c r="D1121" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1122">
+      <c r="A1122" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1122" t="inlineStr">
+        <is>
+          <t>sensorMagneticField</t>
+        </is>
+      </c>
+      <c r="C1122" t="inlineStr">
+        <is>
+          <t>acts</t>
+        </is>
+      </c>
+      <c r="D1122" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1123">
+      <c r="A1123" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1123" t="inlineStr">
+        <is>
+          <t>jointAngle</t>
+        </is>
+      </c>
+      <c r="C1123" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D1123" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1124">
+      <c r="A1124" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1124" t="inlineStr">
+        <is>
+          <t>jointAngle</t>
+        </is>
+      </c>
+      <c r="C1124" t="inlineStr">
+        <is>
+          <t>overall</t>
+        </is>
+      </c>
+      <c r="D1124" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1125">
+      <c r="A1125" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1125" t="inlineStr">
+        <is>
+          <t>jointAngle</t>
+        </is>
+      </c>
+      <c r="C1125" t="inlineStr">
+        <is>
+          <t>acts</t>
+        </is>
+      </c>
+      <c r="D1125" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1126">
+      <c r="A1126" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1126" t="inlineStr">
+        <is>
+          <t>AD</t>
+        </is>
+      </c>
+      <c r="C1126" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D1126" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="1127">
+      <c r="A1127" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1127" t="inlineStr">
+        <is>
+          <t>AD</t>
+        </is>
+      </c>
+      <c r="C1127" t="inlineStr">
+        <is>
+          <t>overall</t>
+        </is>
+      </c>
+      <c r="D1127" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="1128">
+      <c r="A1128" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1128" t="inlineStr">
+        <is>
+          <t>AD</t>
+        </is>
+      </c>
+      <c r="C1128" t="inlineStr">
+        <is>
+          <t>acts</t>
+        </is>
+      </c>
+      <c r="D1128" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="1129">
+      <c r="A1129" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1129" t="inlineStr">
+        <is>
+          <t>jointAngle</t>
+        </is>
+      </c>
+      <c r="C1129" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D1129" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1130">
+      <c r="A1130" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1130" t="inlineStr">
+        <is>
+          <t>jointAngle</t>
+        </is>
+      </c>
+      <c r="C1130" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D1130" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1131">
+      <c r="A1131" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1131" t="inlineStr">
+        <is>
+          <t>jointAngle</t>
+        </is>
+      </c>
+      <c r="C1131" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D1131" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1132">
+      <c r="A1132" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1132" t="inlineStr">
+        <is>
+          <t>jointAngle</t>
+        </is>
+      </c>
+      <c r="C1132" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D1132" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1133">
+      <c r="A1133" t="inlineStr">
+        <is>
+          <t>allmatfiles</t>
+        </is>
+      </c>
+      <c r="B1133" t="inlineStr">
+        <is>
+          <t>jointAngle</t>
+        </is>
+      </c>
+      <c r="C1133" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D1133" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1134">
+      <c r="A1134" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1134" t="inlineStr">
+        <is>
+          <t>jointAngle</t>
+        </is>
+      </c>
+      <c r="C1134" t="inlineStr">
+        <is>
+          <t>overall</t>
+        </is>
+      </c>
+      <c r="D1134" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1135">
+      <c r="A1135" t="inlineStr">
+        <is>
+          <t>allmatfiles</t>
+        </is>
+      </c>
+      <c r="B1135" t="inlineStr">
+        <is>
+          <t>jointAngle</t>
+        </is>
+      </c>
+      <c r="C1135" t="inlineStr">
+        <is>
+          <t>overall</t>
+        </is>
+      </c>
+      <c r="D1135" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1136">
+      <c r="A1136" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1136" t="inlineStr">
+        <is>
+          <t>jointAngle</t>
+        </is>
+      </c>
+      <c r="C1136" t="inlineStr">
+        <is>
+          <t>acts</t>
+        </is>
+      </c>
+      <c r="D1136" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1137">
+      <c r="A1137" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1137" t="inlineStr">
+        <is>
+          <t>jointAngle</t>
+        </is>
+      </c>
+      <c r="C1137" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D1137" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1138">
+      <c r="A1138" t="inlineStr">
+        <is>
+          <t>allmatfiles</t>
+        </is>
+      </c>
+      <c r="B1138" t="inlineStr">
+        <is>
+          <t>jointAngle</t>
+        </is>
+      </c>
+      <c r="C1138" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D1138" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1139">
+      <c r="A1139" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1139" t="inlineStr">
+        <is>
+          <t>jointAngle</t>
+        </is>
+      </c>
+      <c r="C1139" t="inlineStr">
+        <is>
+          <t>overall</t>
+        </is>
+      </c>
+      <c r="D1139" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1140">
+      <c r="A1140" t="inlineStr">
+        <is>
+          <t>allmatfiles</t>
+        </is>
+      </c>
+      <c r="B1140" t="inlineStr">
+        <is>
+          <t>jointAngle</t>
+        </is>
+      </c>
+      <c r="C1140" t="inlineStr">
+        <is>
+          <t>overall</t>
+        </is>
+      </c>
+      <c r="D1140" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1141">
+      <c r="A1141" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1141" t="inlineStr">
+        <is>
+          <t>jointAngle</t>
+        </is>
+      </c>
+      <c r="C1141" t="inlineStr">
+        <is>
+          <t>acts</t>
+        </is>
+      </c>
+      <c r="D1141" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1142">
+      <c r="A1142" t="inlineStr">
+        <is>
+          <t>allmatfiles</t>
+        </is>
+      </c>
+      <c r="B1142" t="inlineStr">
+        <is>
+          <t>jointAngle</t>
+        </is>
+      </c>
+      <c r="C1142" t="inlineStr">
+        <is>
+          <t>acts</t>
+        </is>
+      </c>
+      <c r="D1142" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1143">
+      <c r="A1143" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1143" t="inlineStr">
+        <is>
+          <t>jointAngle</t>
+        </is>
+      </c>
+      <c r="C1143" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D1143" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1144">
+      <c r="A1144" t="inlineStr">
+        <is>
+          <t>allmatfiles</t>
+        </is>
+      </c>
+      <c r="B1144" t="inlineStr">
+        <is>
+          <t>jointAngle</t>
+        </is>
+      </c>
+      <c r="C1144" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D1144" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1145">
+      <c r="A1145" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1145" t="inlineStr">
+        <is>
+          <t>jointAngle</t>
+        </is>
+      </c>
+      <c r="C1145" t="inlineStr">
+        <is>
+          <t>overall</t>
+        </is>
+      </c>
+      <c r="D1145" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1146">
+      <c r="A1146" t="inlineStr">
+        <is>
+          <t>allmatfiles</t>
+        </is>
+      </c>
+      <c r="B1146" t="inlineStr">
+        <is>
+          <t>jointAngle</t>
+        </is>
+      </c>
+      <c r="C1146" t="inlineStr">
+        <is>
+          <t>overall</t>
+        </is>
+      </c>
+      <c r="D1146" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1147">
+      <c r="A1147" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1147" t="inlineStr">
+        <is>
+          <t>jointAngle</t>
+        </is>
+      </c>
+      <c r="C1147" t="inlineStr">
+        <is>
+          <t>acts</t>
+        </is>
+      </c>
+      <c r="D1147" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1148">
+      <c r="A1148" t="inlineStr">
+        <is>
+          <t>allmatfiles</t>
+        </is>
+      </c>
+      <c r="B1148" t="inlineStr">
+        <is>
+          <t>jointAngle</t>
+        </is>
+      </c>
+      <c r="C1148" t="inlineStr">
+        <is>
+          <t>acts</t>
+        </is>
+      </c>
+      <c r="D1148" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1149">
+      <c r="A1149" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1149" t="inlineStr">
+        <is>
+          <t>jointAngle</t>
+        </is>
+      </c>
+      <c r="C1149" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D1149" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1150">
+      <c r="A1150" t="inlineStr">
+        <is>
+          <t>allmatfiles</t>
+        </is>
+      </c>
+      <c r="B1150" t="inlineStr">
+        <is>
+          <t>jointAngle</t>
+        </is>
+      </c>
+      <c r="C1150" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D1150" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1151">
+      <c r="A1151" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1151" t="inlineStr">
+        <is>
+          <t>jointAngle</t>
+        </is>
+      </c>
+      <c r="C1151" t="inlineStr">
+        <is>
+          <t>overall</t>
+        </is>
+      </c>
+      <c r="D1151" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1152">
+      <c r="A1152" t="inlineStr">
+        <is>
+          <t>allmatfiles</t>
+        </is>
+      </c>
+      <c r="B1152" t="inlineStr">
+        <is>
+          <t>jointAngle</t>
+        </is>
+      </c>
+      <c r="C1152" t="inlineStr">
+        <is>
+          <t>overall</t>
+        </is>
+      </c>
+      <c r="D1152" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1153">
+      <c r="A1153" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1153" t="inlineStr">
+        <is>
+          <t>jointAngle</t>
+        </is>
+      </c>
+      <c r="C1153" t="inlineStr">
+        <is>
+          <t>acts</t>
+        </is>
+      </c>
+      <c r="D1153" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1154">
+      <c r="A1154" t="inlineStr">
+        <is>
+          <t>allmatfiles</t>
+        </is>
+      </c>
+      <c r="B1154" t="inlineStr">
+        <is>
+          <t>jointAngle</t>
+        </is>
+      </c>
+      <c r="C1154" t="inlineStr">
+        <is>
+          <t>acts</t>
+        </is>
+      </c>
+      <c r="D1154" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1155">
+      <c r="A1155" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1155" t="inlineStr">
+        <is>
+          <t>jointAngle</t>
+        </is>
+      </c>
+      <c r="C1155" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D1155" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1156">
+      <c r="A1156" t="inlineStr">
+        <is>
+          <t>allmatfiles</t>
+        </is>
+      </c>
+      <c r="B1156" t="inlineStr">
+        <is>
+          <t>jointAngle</t>
+        </is>
+      </c>
+      <c r="C1156" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D1156" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1157">
+      <c r="A1157" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1157" t="inlineStr">
+        <is>
+          <t>jointAngle</t>
+        </is>
+      </c>
+      <c r="C1157" t="inlineStr">
+        <is>
+          <t>overall</t>
+        </is>
+      </c>
+      <c r="D1157" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1158">
+      <c r="A1158" t="inlineStr">
+        <is>
+          <t>allmatfiles</t>
+        </is>
+      </c>
+      <c r="B1158" t="inlineStr">
+        <is>
+          <t>jointAngle</t>
+        </is>
+      </c>
+      <c r="C1158" t="inlineStr">
+        <is>
+          <t>overall</t>
+        </is>
+      </c>
+      <c r="D1158" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1159">
+      <c r="A1159" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1159" t="inlineStr">
+        <is>
+          <t>jointAngle</t>
+        </is>
+      </c>
+      <c r="C1159" t="inlineStr">
+        <is>
+          <t>acts</t>
+        </is>
+      </c>
+      <c r="D1159" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1160">
+      <c r="A1160" t="inlineStr">
+        <is>
+          <t>allmatfiles</t>
+        </is>
+      </c>
+      <c r="B1160" t="inlineStr">
+        <is>
+          <t>jointAngle</t>
+        </is>
+      </c>
+      <c r="C1160" t="inlineStr">
+        <is>
+          <t>acts</t>
+        </is>
+      </c>
+      <c r="D1160" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1161">
+      <c r="A1161" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1161" t="inlineStr">
+        <is>
+          <t>jointAngle</t>
+        </is>
+      </c>
+      <c r="C1161" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D1161" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1162">
+      <c r="A1162" t="inlineStr">
+        <is>
+          <t>allmatfiles</t>
+        </is>
+      </c>
+      <c r="B1162" t="inlineStr">
+        <is>
+          <t>jointAngle</t>
+        </is>
+      </c>
+      <c r="C1162" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D1162" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1163">
+      <c r="A1163" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1163" t="inlineStr">
+        <is>
+          <t>jointAngle</t>
+        </is>
+      </c>
+      <c r="C1163" t="inlineStr">
+        <is>
+          <t>overall</t>
+        </is>
+      </c>
+      <c r="D1163" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1164">
+      <c r="A1164" t="inlineStr">
+        <is>
+          <t>allmatfiles</t>
+        </is>
+      </c>
+      <c r="B1164" t="inlineStr">
+        <is>
+          <t>jointAngle</t>
+        </is>
+      </c>
+      <c r="C1164" t="inlineStr">
+        <is>
+          <t>overall</t>
+        </is>
+      </c>
+      <c r="D1164" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1165">
+      <c r="A1165" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1165" t="inlineStr">
+        <is>
+          <t>jointAngle</t>
+        </is>
+      </c>
+      <c r="C1165" t="inlineStr">
+        <is>
+          <t>acts</t>
+        </is>
+      </c>
+      <c r="D1165" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1166">
+      <c r="A1166" t="inlineStr">
+        <is>
+          <t>allmatfiles</t>
+        </is>
+      </c>
+      <c r="B1166" t="inlineStr">
+        <is>
+          <t>jointAngle</t>
+        </is>
+      </c>
+      <c r="C1166" t="inlineStr">
+        <is>
+          <t>acts</t>
+        </is>
+      </c>
+      <c r="D1166" t="n">
+        <v>60</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>

<commit_message>
Added several report sections including bibliography, directories overview, and added to experiments and results discussion, with adding the necessary batch files to run the model prediction sets and making necessary changes to 'source' files.
</commit_message>
<xml_diff>
--- a/documentation/model_shapes.xlsx
+++ b/documentation/model_shapes.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D1166"/>
+  <dimension ref="A1:D1275"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -23688,6 +23688,2186 @@
         <v>60</v>
       </c>
     </row>
+    <row r="1167">
+      <c r="A1167" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1167" t="inlineStr">
+        <is>
+          <t>jointAngle</t>
+        </is>
+      </c>
+      <c r="C1167" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D1167" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1168">
+      <c r="A1168" t="inlineStr">
+        <is>
+          <t>allmatfiles</t>
+        </is>
+      </c>
+      <c r="B1168" t="inlineStr">
+        <is>
+          <t>jointAngle</t>
+        </is>
+      </c>
+      <c r="C1168" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D1168" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1169">
+      <c r="A1169" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1169" t="inlineStr">
+        <is>
+          <t>jointAngle</t>
+        </is>
+      </c>
+      <c r="C1169" t="inlineStr">
+        <is>
+          <t>overall</t>
+        </is>
+      </c>
+      <c r="D1169" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1170">
+      <c r="A1170" t="inlineStr">
+        <is>
+          <t>allmatfiles</t>
+        </is>
+      </c>
+      <c r="B1170" t="inlineStr">
+        <is>
+          <t>jointAngle</t>
+        </is>
+      </c>
+      <c r="C1170" t="inlineStr">
+        <is>
+          <t>overall</t>
+        </is>
+      </c>
+      <c r="D1170" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1171">
+      <c r="A1171" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1171" t="inlineStr">
+        <is>
+          <t>jointAngle</t>
+        </is>
+      </c>
+      <c r="C1171" t="inlineStr">
+        <is>
+          <t>acts</t>
+        </is>
+      </c>
+      <c r="D1171" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1172">
+      <c r="A1172" t="inlineStr">
+        <is>
+          <t>allmatfiles</t>
+        </is>
+      </c>
+      <c r="B1172" t="inlineStr">
+        <is>
+          <t>jointAngle</t>
+        </is>
+      </c>
+      <c r="C1172" t="inlineStr">
+        <is>
+          <t>acts</t>
+        </is>
+      </c>
+      <c r="D1172" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1173">
+      <c r="A1173" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1173" t="inlineStr">
+        <is>
+          <t>jointAngle</t>
+        </is>
+      </c>
+      <c r="C1173" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D1173" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1174">
+      <c r="A1174" t="inlineStr">
+        <is>
+          <t>allmatfiles</t>
+        </is>
+      </c>
+      <c r="B1174" t="inlineStr">
+        <is>
+          <t>jointAngle</t>
+        </is>
+      </c>
+      <c r="C1174" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D1174" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1175">
+      <c r="A1175" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1175" t="inlineStr">
+        <is>
+          <t>jointAngle</t>
+        </is>
+      </c>
+      <c r="C1175" t="inlineStr">
+        <is>
+          <t>overall</t>
+        </is>
+      </c>
+      <c r="D1175" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1176">
+      <c r="A1176" t="inlineStr">
+        <is>
+          <t>allmatfiles</t>
+        </is>
+      </c>
+      <c r="B1176" t="inlineStr">
+        <is>
+          <t>jointAngle</t>
+        </is>
+      </c>
+      <c r="C1176" t="inlineStr">
+        <is>
+          <t>overall</t>
+        </is>
+      </c>
+      <c r="D1176" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1177">
+      <c r="A1177" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1177" t="inlineStr">
+        <is>
+          <t>jointAngle</t>
+        </is>
+      </c>
+      <c r="C1177" t="inlineStr">
+        <is>
+          <t>acts</t>
+        </is>
+      </c>
+      <c r="D1177" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1178">
+      <c r="A1178" t="inlineStr">
+        <is>
+          <t>allmatfiles</t>
+        </is>
+      </c>
+      <c r="B1178" t="inlineStr">
+        <is>
+          <t>jointAngle</t>
+        </is>
+      </c>
+      <c r="C1178" t="inlineStr">
+        <is>
+          <t>acts</t>
+        </is>
+      </c>
+      <c r="D1178" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1179">
+      <c r="A1179" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1179" t="inlineStr">
+        <is>
+          <t>jointAngle</t>
+        </is>
+      </c>
+      <c r="C1179" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D1179" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1180">
+      <c r="A1180" t="inlineStr">
+        <is>
+          <t>allmatfiles</t>
+        </is>
+      </c>
+      <c r="B1180" t="inlineStr">
+        <is>
+          <t>jointAngle</t>
+        </is>
+      </c>
+      <c r="C1180" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D1180" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1181">
+      <c r="A1181" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1181" t="inlineStr">
+        <is>
+          <t>jointAngle</t>
+        </is>
+      </c>
+      <c r="C1181" t="inlineStr">
+        <is>
+          <t>overall</t>
+        </is>
+      </c>
+      <c r="D1181" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1182">
+      <c r="A1182" t="inlineStr">
+        <is>
+          <t>allmatfiles</t>
+        </is>
+      </c>
+      <c r="B1182" t="inlineStr">
+        <is>
+          <t>jointAngle</t>
+        </is>
+      </c>
+      <c r="C1182" t="inlineStr">
+        <is>
+          <t>overall</t>
+        </is>
+      </c>
+      <c r="D1182" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1183">
+      <c r="A1183" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1183" t="inlineStr">
+        <is>
+          <t>jointAngle</t>
+        </is>
+      </c>
+      <c r="C1183" t="inlineStr">
+        <is>
+          <t>acts</t>
+        </is>
+      </c>
+      <c r="D1183" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1184">
+      <c r="A1184" t="inlineStr">
+        <is>
+          <t>allmatfiles</t>
+        </is>
+      </c>
+      <c r="B1184" t="inlineStr">
+        <is>
+          <t>jointAngle</t>
+        </is>
+      </c>
+      <c r="C1184" t="inlineStr">
+        <is>
+          <t>acts</t>
+        </is>
+      </c>
+      <c r="D1184" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1185">
+      <c r="A1185" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1185" t="inlineStr">
+        <is>
+          <t>jointAngle</t>
+        </is>
+      </c>
+      <c r="C1185" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D1185" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1186">
+      <c r="A1186" t="inlineStr">
+        <is>
+          <t>allmatfiles</t>
+        </is>
+      </c>
+      <c r="B1186" t="inlineStr">
+        <is>
+          <t>jointAngle</t>
+        </is>
+      </c>
+      <c r="C1186" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D1186" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1187">
+      <c r="A1187" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1187" t="inlineStr">
+        <is>
+          <t>jointAngle</t>
+        </is>
+      </c>
+      <c r="C1187" t="inlineStr">
+        <is>
+          <t>overall</t>
+        </is>
+      </c>
+      <c r="D1187" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1188">
+      <c r="A1188" t="inlineStr">
+        <is>
+          <t>allmatfiles</t>
+        </is>
+      </c>
+      <c r="B1188" t="inlineStr">
+        <is>
+          <t>jointAngle</t>
+        </is>
+      </c>
+      <c r="C1188" t="inlineStr">
+        <is>
+          <t>overall</t>
+        </is>
+      </c>
+      <c r="D1188" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1189">
+      <c r="A1189" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1189" t="inlineStr">
+        <is>
+          <t>jointAngle</t>
+        </is>
+      </c>
+      <c r="C1189" t="inlineStr">
+        <is>
+          <t>acts</t>
+        </is>
+      </c>
+      <c r="D1189" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1190">
+      <c r="A1190" t="inlineStr">
+        <is>
+          <t>allmatfiles</t>
+        </is>
+      </c>
+      <c r="B1190" t="inlineStr">
+        <is>
+          <t>jointAngle</t>
+        </is>
+      </c>
+      <c r="C1190" t="inlineStr">
+        <is>
+          <t>acts</t>
+        </is>
+      </c>
+      <c r="D1190" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1191">
+      <c r="A1191" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1191" t="inlineStr">
+        <is>
+          <t>jointAngle</t>
+        </is>
+      </c>
+      <c r="C1191" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D1191" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1192">
+      <c r="A1192" t="inlineStr">
+        <is>
+          <t>allmatfiles</t>
+        </is>
+      </c>
+      <c r="B1192" t="inlineStr">
+        <is>
+          <t>jointAngle</t>
+        </is>
+      </c>
+      <c r="C1192" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D1192" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1193">
+      <c r="A1193" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1193" t="inlineStr">
+        <is>
+          <t>jointAngle</t>
+        </is>
+      </c>
+      <c r="C1193" t="inlineStr">
+        <is>
+          <t>overall</t>
+        </is>
+      </c>
+      <c r="D1193" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1194">
+      <c r="A1194" t="inlineStr">
+        <is>
+          <t>allmatfiles</t>
+        </is>
+      </c>
+      <c r="B1194" t="inlineStr">
+        <is>
+          <t>jointAngle</t>
+        </is>
+      </c>
+      <c r="C1194" t="inlineStr">
+        <is>
+          <t>overall</t>
+        </is>
+      </c>
+      <c r="D1194" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1195">
+      <c r="A1195" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1195" t="inlineStr">
+        <is>
+          <t>jointAngle</t>
+        </is>
+      </c>
+      <c r="C1195" t="inlineStr">
+        <is>
+          <t>acts</t>
+        </is>
+      </c>
+      <c r="D1195" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1196">
+      <c r="A1196" t="inlineStr">
+        <is>
+          <t>allmatfiles</t>
+        </is>
+      </c>
+      <c r="B1196" t="inlineStr">
+        <is>
+          <t>jointAngle</t>
+        </is>
+      </c>
+      <c r="C1196" t="inlineStr">
+        <is>
+          <t>acts</t>
+        </is>
+      </c>
+      <c r="D1196" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1197">
+      <c r="A1197" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1197" t="inlineStr">
+        <is>
+          <t>position</t>
+        </is>
+      </c>
+      <c r="C1197" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D1197" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1198">
+      <c r="A1198" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1198" t="inlineStr">
+        <is>
+          <t>position</t>
+        </is>
+      </c>
+      <c r="C1198" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D1198" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1199">
+      <c r="A1199" t="inlineStr">
+        <is>
+          <t>NMB</t>
+        </is>
+      </c>
+      <c r="B1199" t="inlineStr">
+        <is>
+          <t>position</t>
+        </is>
+      </c>
+      <c r="C1199" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D1199" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1200">
+      <c r="A1200" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1200" t="inlineStr">
+        <is>
+          <t>position</t>
+        </is>
+      </c>
+      <c r="C1200" t="inlineStr">
+        <is>
+          <t>overall</t>
+        </is>
+      </c>
+      <c r="D1200" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1201">
+      <c r="A1201" t="inlineStr">
+        <is>
+          <t>NMB</t>
+        </is>
+      </c>
+      <c r="B1201" t="inlineStr">
+        <is>
+          <t>position</t>
+        </is>
+      </c>
+      <c r="C1201" t="inlineStr">
+        <is>
+          <t>overall</t>
+        </is>
+      </c>
+      <c r="D1201" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1202">
+      <c r="A1202" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1202" t="inlineStr">
+        <is>
+          <t>position</t>
+        </is>
+      </c>
+      <c r="C1202" t="inlineStr">
+        <is>
+          <t>acts</t>
+        </is>
+      </c>
+      <c r="D1202" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1203">
+      <c r="A1203" t="inlineStr">
+        <is>
+          <t>NMB</t>
+        </is>
+      </c>
+      <c r="B1203" t="inlineStr">
+        <is>
+          <t>position</t>
+        </is>
+      </c>
+      <c r="C1203" t="inlineStr">
+        <is>
+          <t>acts</t>
+        </is>
+      </c>
+      <c r="D1203" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1204">
+      <c r="A1204" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1204" t="inlineStr">
+        <is>
+          <t>sensorMagneticField</t>
+        </is>
+      </c>
+      <c r="C1204" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D1204" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1205">
+      <c r="A1205" t="inlineStr">
+        <is>
+          <t>NMB</t>
+        </is>
+      </c>
+      <c r="B1205" t="inlineStr">
+        <is>
+          <t>sensorMagneticField</t>
+        </is>
+      </c>
+      <c r="C1205" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D1205" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1206">
+      <c r="A1206" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1206" t="inlineStr">
+        <is>
+          <t>sensorMagneticField</t>
+        </is>
+      </c>
+      <c r="C1206" t="inlineStr">
+        <is>
+          <t>overall</t>
+        </is>
+      </c>
+      <c r="D1206" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1207">
+      <c r="A1207" t="inlineStr">
+        <is>
+          <t>NMB</t>
+        </is>
+      </c>
+      <c r="B1207" t="inlineStr">
+        <is>
+          <t>sensorMagneticField</t>
+        </is>
+      </c>
+      <c r="C1207" t="inlineStr">
+        <is>
+          <t>overall</t>
+        </is>
+      </c>
+      <c r="D1207" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1208">
+      <c r="A1208" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1208" t="inlineStr">
+        <is>
+          <t>sensorMagneticField</t>
+        </is>
+      </c>
+      <c r="C1208" t="inlineStr">
+        <is>
+          <t>acts</t>
+        </is>
+      </c>
+      <c r="D1208" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1209">
+      <c r="A1209" t="inlineStr">
+        <is>
+          <t>NMB</t>
+        </is>
+      </c>
+      <c r="B1209" t="inlineStr">
+        <is>
+          <t>sensorMagneticField</t>
+        </is>
+      </c>
+      <c r="C1209" t="inlineStr">
+        <is>
+          <t>acts</t>
+        </is>
+      </c>
+      <c r="D1209" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1210">
+      <c r="A1210" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1210" t="inlineStr">
+        <is>
+          <t>jointAngle</t>
+        </is>
+      </c>
+      <c r="C1210" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D1210" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1211">
+      <c r="A1211" t="inlineStr">
+        <is>
+          <t>NMB</t>
+        </is>
+      </c>
+      <c r="B1211" t="inlineStr">
+        <is>
+          <t>jointAngle</t>
+        </is>
+      </c>
+      <c r="C1211" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D1211" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1212">
+      <c r="A1212" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1212" t="inlineStr">
+        <is>
+          <t>jointAngle</t>
+        </is>
+      </c>
+      <c r="C1212" t="inlineStr">
+        <is>
+          <t>overall</t>
+        </is>
+      </c>
+      <c r="D1212" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1213">
+      <c r="A1213" t="inlineStr">
+        <is>
+          <t>NMB</t>
+        </is>
+      </c>
+      <c r="B1213" t="inlineStr">
+        <is>
+          <t>jointAngle</t>
+        </is>
+      </c>
+      <c r="C1213" t="inlineStr">
+        <is>
+          <t>overall</t>
+        </is>
+      </c>
+      <c r="D1213" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1214">
+      <c r="A1214" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1214" t="inlineStr">
+        <is>
+          <t>jointAngle</t>
+        </is>
+      </c>
+      <c r="C1214" t="inlineStr">
+        <is>
+          <t>acts</t>
+        </is>
+      </c>
+      <c r="D1214" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1215">
+      <c r="A1215" t="inlineStr">
+        <is>
+          <t>NMB</t>
+        </is>
+      </c>
+      <c r="B1215" t="inlineStr">
+        <is>
+          <t>jointAngle</t>
+        </is>
+      </c>
+      <c r="C1215" t="inlineStr">
+        <is>
+          <t>acts</t>
+        </is>
+      </c>
+      <c r="D1215" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1216">
+      <c r="A1216" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1216" t="inlineStr">
+        <is>
+          <t>AD</t>
+        </is>
+      </c>
+      <c r="C1216" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D1216" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1217">
+      <c r="A1217" t="inlineStr">
+        <is>
+          <t>NMB</t>
+        </is>
+      </c>
+      <c r="B1217" t="inlineStr">
+        <is>
+          <t>AD</t>
+        </is>
+      </c>
+      <c r="C1217" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D1217" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1218">
+      <c r="A1218" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1218" t="inlineStr">
+        <is>
+          <t>AD</t>
+        </is>
+      </c>
+      <c r="C1218" t="inlineStr">
+        <is>
+          <t>overall</t>
+        </is>
+      </c>
+      <c r="D1218" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1219">
+      <c r="A1219" t="inlineStr">
+        <is>
+          <t>NMB</t>
+        </is>
+      </c>
+      <c r="B1219" t="inlineStr">
+        <is>
+          <t>AD</t>
+        </is>
+      </c>
+      <c r="C1219" t="inlineStr">
+        <is>
+          <t>overall</t>
+        </is>
+      </c>
+      <c r="D1219" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1220">
+      <c r="A1220" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1220" t="inlineStr">
+        <is>
+          <t>AD</t>
+        </is>
+      </c>
+      <c r="C1220" t="inlineStr">
+        <is>
+          <t>acts</t>
+        </is>
+      </c>
+      <c r="D1220" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1221">
+      <c r="A1221" t="inlineStr">
+        <is>
+          <t>NMB</t>
+        </is>
+      </c>
+      <c r="B1221" t="inlineStr">
+        <is>
+          <t>AD</t>
+        </is>
+      </c>
+      <c r="C1221" t="inlineStr">
+        <is>
+          <t>acts</t>
+        </is>
+      </c>
+      <c r="D1221" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1222">
+      <c r="A1222" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1222" t="inlineStr">
+        <is>
+          <t>position</t>
+        </is>
+      </c>
+      <c r="C1222" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D1222" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1223">
+      <c r="A1223" t="inlineStr">
+        <is>
+          <t>NMB</t>
+        </is>
+      </c>
+      <c r="B1223" t="inlineStr">
+        <is>
+          <t>position</t>
+        </is>
+      </c>
+      <c r="C1223" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D1223" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1224">
+      <c r="A1224" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1224" t="inlineStr">
+        <is>
+          <t>position</t>
+        </is>
+      </c>
+      <c r="C1224" t="inlineStr">
+        <is>
+          <t>overall</t>
+        </is>
+      </c>
+      <c r="D1224" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1225">
+      <c r="A1225" t="inlineStr">
+        <is>
+          <t>NMB</t>
+        </is>
+      </c>
+      <c r="B1225" t="inlineStr">
+        <is>
+          <t>position</t>
+        </is>
+      </c>
+      <c r="C1225" t="inlineStr">
+        <is>
+          <t>overall</t>
+        </is>
+      </c>
+      <c r="D1225" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1226">
+      <c r="A1226" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1226" t="inlineStr">
+        <is>
+          <t>position</t>
+        </is>
+      </c>
+      <c r="C1226" t="inlineStr">
+        <is>
+          <t>acts</t>
+        </is>
+      </c>
+      <c r="D1226" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1227">
+      <c r="A1227" t="inlineStr">
+        <is>
+          <t>NMB</t>
+        </is>
+      </c>
+      <c r="B1227" t="inlineStr">
+        <is>
+          <t>position</t>
+        </is>
+      </c>
+      <c r="C1227" t="inlineStr">
+        <is>
+          <t>acts</t>
+        </is>
+      </c>
+      <c r="D1227" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1228">
+      <c r="A1228" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1228" t="inlineStr">
+        <is>
+          <t>sensorMagneticField</t>
+        </is>
+      </c>
+      <c r="C1228" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D1228" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1229">
+      <c r="A1229" t="inlineStr">
+        <is>
+          <t>NMB</t>
+        </is>
+      </c>
+      <c r="B1229" t="inlineStr">
+        <is>
+          <t>sensorMagneticField</t>
+        </is>
+      </c>
+      <c r="C1229" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D1229" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1230">
+      <c r="A1230" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1230" t="inlineStr">
+        <is>
+          <t>sensorMagneticField</t>
+        </is>
+      </c>
+      <c r="C1230" t="inlineStr">
+        <is>
+          <t>overall</t>
+        </is>
+      </c>
+      <c r="D1230" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1231">
+      <c r="A1231" t="inlineStr">
+        <is>
+          <t>NMB</t>
+        </is>
+      </c>
+      <c r="B1231" t="inlineStr">
+        <is>
+          <t>sensorMagneticField</t>
+        </is>
+      </c>
+      <c r="C1231" t="inlineStr">
+        <is>
+          <t>overall</t>
+        </is>
+      </c>
+      <c r="D1231" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1232">
+      <c r="A1232" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1232" t="inlineStr">
+        <is>
+          <t>sensorMagneticField</t>
+        </is>
+      </c>
+      <c r="C1232" t="inlineStr">
+        <is>
+          <t>acts</t>
+        </is>
+      </c>
+      <c r="D1232" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1233">
+      <c r="A1233" t="inlineStr">
+        <is>
+          <t>NMB</t>
+        </is>
+      </c>
+      <c r="B1233" t="inlineStr">
+        <is>
+          <t>sensorMagneticField</t>
+        </is>
+      </c>
+      <c r="C1233" t="inlineStr">
+        <is>
+          <t>acts</t>
+        </is>
+      </c>
+      <c r="D1233" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1234">
+      <c r="A1234" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1234" t="inlineStr">
+        <is>
+          <t>jointAngle</t>
+        </is>
+      </c>
+      <c r="C1234" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D1234" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1235">
+      <c r="A1235" t="inlineStr">
+        <is>
+          <t>NMB</t>
+        </is>
+      </c>
+      <c r="B1235" t="inlineStr">
+        <is>
+          <t>jointAngle</t>
+        </is>
+      </c>
+      <c r="C1235" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D1235" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1236">
+      <c r="A1236" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1236" t="inlineStr">
+        <is>
+          <t>jointAngle</t>
+        </is>
+      </c>
+      <c r="C1236" t="inlineStr">
+        <is>
+          <t>overall</t>
+        </is>
+      </c>
+      <c r="D1236" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1237">
+      <c r="A1237" t="inlineStr">
+        <is>
+          <t>NMB</t>
+        </is>
+      </c>
+      <c r="B1237" t="inlineStr">
+        <is>
+          <t>jointAngle</t>
+        </is>
+      </c>
+      <c r="C1237" t="inlineStr">
+        <is>
+          <t>overall</t>
+        </is>
+      </c>
+      <c r="D1237" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1238">
+      <c r="A1238" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1238" t="inlineStr">
+        <is>
+          <t>jointAngle</t>
+        </is>
+      </c>
+      <c r="C1238" t="inlineStr">
+        <is>
+          <t>acts</t>
+        </is>
+      </c>
+      <c r="D1238" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1239">
+      <c r="A1239" t="inlineStr">
+        <is>
+          <t>NMB</t>
+        </is>
+      </c>
+      <c r="B1239" t="inlineStr">
+        <is>
+          <t>jointAngle</t>
+        </is>
+      </c>
+      <c r="C1239" t="inlineStr">
+        <is>
+          <t>acts</t>
+        </is>
+      </c>
+      <c r="D1239" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1240">
+      <c r="A1240" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1240" t="inlineStr">
+        <is>
+          <t>AD</t>
+        </is>
+      </c>
+      <c r="C1240" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D1240" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1241">
+      <c r="A1241" t="inlineStr">
+        <is>
+          <t>NMB</t>
+        </is>
+      </c>
+      <c r="B1241" t="inlineStr">
+        <is>
+          <t>AD</t>
+        </is>
+      </c>
+      <c r="C1241" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D1241" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1242">
+      <c r="A1242" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1242" t="inlineStr">
+        <is>
+          <t>AD</t>
+        </is>
+      </c>
+      <c r="C1242" t="inlineStr">
+        <is>
+          <t>overall</t>
+        </is>
+      </c>
+      <c r="D1242" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1243">
+      <c r="A1243" t="inlineStr">
+        <is>
+          <t>NMB</t>
+        </is>
+      </c>
+      <c r="B1243" t="inlineStr">
+        <is>
+          <t>AD</t>
+        </is>
+      </c>
+      <c r="C1243" t="inlineStr">
+        <is>
+          <t>overall</t>
+        </is>
+      </c>
+      <c r="D1243" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1244">
+      <c r="A1244" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1244" t="inlineStr">
+        <is>
+          <t>AD</t>
+        </is>
+      </c>
+      <c r="C1244" t="inlineStr">
+        <is>
+          <t>acts</t>
+        </is>
+      </c>
+      <c r="D1244" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1245">
+      <c r="A1245" t="inlineStr">
+        <is>
+          <t>NMB</t>
+        </is>
+      </c>
+      <c r="B1245" t="inlineStr">
+        <is>
+          <t>AD</t>
+        </is>
+      </c>
+      <c r="C1245" t="inlineStr">
+        <is>
+          <t>acts</t>
+        </is>
+      </c>
+      <c r="D1245" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1246">
+      <c r="A1246" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1246" t="inlineStr">
+        <is>
+          <t>position</t>
+        </is>
+      </c>
+      <c r="C1246" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D1246" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1247">
+      <c r="A1247" t="inlineStr">
+        <is>
+          <t>NMB</t>
+        </is>
+      </c>
+      <c r="B1247" t="inlineStr">
+        <is>
+          <t>position</t>
+        </is>
+      </c>
+      <c r="C1247" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D1247" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1248">
+      <c r="A1248" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1248" t="inlineStr">
+        <is>
+          <t>position</t>
+        </is>
+      </c>
+      <c r="C1248" t="inlineStr">
+        <is>
+          <t>overall</t>
+        </is>
+      </c>
+      <c r="D1248" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1249">
+      <c r="A1249" t="inlineStr">
+        <is>
+          <t>NMB</t>
+        </is>
+      </c>
+      <c r="B1249" t="inlineStr">
+        <is>
+          <t>position</t>
+        </is>
+      </c>
+      <c r="C1249" t="inlineStr">
+        <is>
+          <t>overall</t>
+        </is>
+      </c>
+      <c r="D1249" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1250">
+      <c r="A1250" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1250" t="inlineStr">
+        <is>
+          <t>position</t>
+        </is>
+      </c>
+      <c r="C1250" t="inlineStr">
+        <is>
+          <t>acts</t>
+        </is>
+      </c>
+      <c r="D1250" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1251">
+      <c r="A1251" t="inlineStr">
+        <is>
+          <t>NMB</t>
+        </is>
+      </c>
+      <c r="B1251" t="inlineStr">
+        <is>
+          <t>position</t>
+        </is>
+      </c>
+      <c r="C1251" t="inlineStr">
+        <is>
+          <t>acts</t>
+        </is>
+      </c>
+      <c r="D1251" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1252">
+      <c r="A1252" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1252" t="inlineStr">
+        <is>
+          <t>sensorMagneticField</t>
+        </is>
+      </c>
+      <c r="C1252" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D1252" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1253">
+      <c r="A1253" t="inlineStr">
+        <is>
+          <t>NMB</t>
+        </is>
+      </c>
+      <c r="B1253" t="inlineStr">
+        <is>
+          <t>sensorMagneticField</t>
+        </is>
+      </c>
+      <c r="C1253" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D1253" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1254">
+      <c r="A1254" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1254" t="inlineStr">
+        <is>
+          <t>sensorMagneticField</t>
+        </is>
+      </c>
+      <c r="C1254" t="inlineStr">
+        <is>
+          <t>overall</t>
+        </is>
+      </c>
+      <c r="D1254" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1255">
+      <c r="A1255" t="inlineStr">
+        <is>
+          <t>NMB</t>
+        </is>
+      </c>
+      <c r="B1255" t="inlineStr">
+        <is>
+          <t>sensorMagneticField</t>
+        </is>
+      </c>
+      <c r="C1255" t="inlineStr">
+        <is>
+          <t>overall</t>
+        </is>
+      </c>
+      <c r="D1255" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1256">
+      <c r="A1256" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1256" t="inlineStr">
+        <is>
+          <t>sensorMagneticField</t>
+        </is>
+      </c>
+      <c r="C1256" t="inlineStr">
+        <is>
+          <t>acts</t>
+        </is>
+      </c>
+      <c r="D1256" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1257">
+      <c r="A1257" t="inlineStr">
+        <is>
+          <t>NMB</t>
+        </is>
+      </c>
+      <c r="B1257" t="inlineStr">
+        <is>
+          <t>sensorMagneticField</t>
+        </is>
+      </c>
+      <c r="C1257" t="inlineStr">
+        <is>
+          <t>acts</t>
+        </is>
+      </c>
+      <c r="D1257" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1258">
+      <c r="A1258" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1258" t="inlineStr">
+        <is>
+          <t>jointAngle</t>
+        </is>
+      </c>
+      <c r="C1258" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D1258" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1259">
+      <c r="A1259" t="inlineStr">
+        <is>
+          <t>NMB</t>
+        </is>
+      </c>
+      <c r="B1259" t="inlineStr">
+        <is>
+          <t>jointAngle</t>
+        </is>
+      </c>
+      <c r="C1259" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D1259" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1260">
+      <c r="A1260" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1260" t="inlineStr">
+        <is>
+          <t>jointAngle</t>
+        </is>
+      </c>
+      <c r="C1260" t="inlineStr">
+        <is>
+          <t>overall</t>
+        </is>
+      </c>
+      <c r="D1260" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1261">
+      <c r="A1261" t="inlineStr">
+        <is>
+          <t>NMB</t>
+        </is>
+      </c>
+      <c r="B1261" t="inlineStr">
+        <is>
+          <t>jointAngle</t>
+        </is>
+      </c>
+      <c r="C1261" t="inlineStr">
+        <is>
+          <t>overall</t>
+        </is>
+      </c>
+      <c r="D1261" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1262">
+      <c r="A1262" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1262" t="inlineStr">
+        <is>
+          <t>jointAngle</t>
+        </is>
+      </c>
+      <c r="C1262" t="inlineStr">
+        <is>
+          <t>acts</t>
+        </is>
+      </c>
+      <c r="D1262" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1263">
+      <c r="A1263" t="inlineStr">
+        <is>
+          <t>NMB</t>
+        </is>
+      </c>
+      <c r="B1263" t="inlineStr">
+        <is>
+          <t>jointAngle</t>
+        </is>
+      </c>
+      <c r="C1263" t="inlineStr">
+        <is>
+          <t>acts</t>
+        </is>
+      </c>
+      <c r="D1263" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1264">
+      <c r="A1264" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1264" t="inlineStr">
+        <is>
+          <t>AD</t>
+        </is>
+      </c>
+      <c r="C1264" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D1264" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1265">
+      <c r="A1265" t="inlineStr">
+        <is>
+          <t>NMB</t>
+        </is>
+      </c>
+      <c r="B1265" t="inlineStr">
+        <is>
+          <t>AD</t>
+        </is>
+      </c>
+      <c r="C1265" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D1265" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1266">
+      <c r="A1266" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1266" t="inlineStr">
+        <is>
+          <t>AD</t>
+        </is>
+      </c>
+      <c r="C1266" t="inlineStr">
+        <is>
+          <t>overall</t>
+        </is>
+      </c>
+      <c r="D1266" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1267">
+      <c r="A1267" t="inlineStr">
+        <is>
+          <t>NMB</t>
+        </is>
+      </c>
+      <c r="B1267" t="inlineStr">
+        <is>
+          <t>AD</t>
+        </is>
+      </c>
+      <c r="C1267" t="inlineStr">
+        <is>
+          <t>overall</t>
+        </is>
+      </c>
+      <c r="D1267" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1268">
+      <c r="A1268" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1268" t="inlineStr">
+        <is>
+          <t>AD</t>
+        </is>
+      </c>
+      <c r="C1268" t="inlineStr">
+        <is>
+          <t>acts</t>
+        </is>
+      </c>
+      <c r="D1268" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1269">
+      <c r="A1269" t="inlineStr">
+        <is>
+          <t>NMB</t>
+        </is>
+      </c>
+      <c r="B1269" t="inlineStr">
+        <is>
+          <t>AD</t>
+        </is>
+      </c>
+      <c r="C1269" t="inlineStr">
+        <is>
+          <t>acts</t>
+        </is>
+      </c>
+      <c r="D1269" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1270">
+      <c r="A1270" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1270" t="inlineStr">
+        <is>
+          <t>position</t>
+        </is>
+      </c>
+      <c r="C1270" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D1270" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1271">
+      <c r="A1271" t="inlineStr">
+        <is>
+          <t>NMB</t>
+        </is>
+      </c>
+      <c r="B1271" t="inlineStr">
+        <is>
+          <t>position</t>
+        </is>
+      </c>
+      <c r="C1271" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D1271" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1272">
+      <c r="A1272" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1272" t="inlineStr">
+        <is>
+          <t>position</t>
+        </is>
+      </c>
+      <c r="C1272" t="inlineStr">
+        <is>
+          <t>overall</t>
+        </is>
+      </c>
+      <c r="D1272" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1273">
+      <c r="A1273" t="inlineStr">
+        <is>
+          <t>NMB</t>
+        </is>
+      </c>
+      <c r="B1273" t="inlineStr">
+        <is>
+          <t>position</t>
+        </is>
+      </c>
+      <c r="C1273" t="inlineStr">
+        <is>
+          <t>overall</t>
+        </is>
+      </c>
+      <c r="D1273" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1274">
+      <c r="A1274" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1274" t="inlineStr">
+        <is>
+          <t>position</t>
+        </is>
+      </c>
+      <c r="C1274" t="inlineStr">
+        <is>
+          <t>acts</t>
+        </is>
+      </c>
+      <c r="D1274" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1275">
+      <c r="A1275" t="inlineStr">
+        <is>
+          <t>NMB</t>
+        </is>
+      </c>
+      <c r="B1275" t="inlineStr">
+        <is>
+          <t>position</t>
+        </is>
+      </c>
+      <c r="C1275" t="inlineStr">
+        <is>
+          <t>acts</t>
+        </is>
+      </c>
+      <c r="D1275" t="n">
+        <v>60</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>

<commit_message>
Completed more model predictions sets, modified 'source' Python files to work with these, created the 'assess_nsaaV2_file.cmd' and 'file_mover.py' files, added more to experiment and results discussion, and added a report parts on DMD background and an RNN overview.
</commit_message>
<xml_diff>
--- a/documentation/model_shapes.xlsx
+++ b/documentation/model_shapes.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D1275"/>
+  <dimension ref="A1:D1375"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -25868,6 +25868,2006 @@
         <v>60</v>
       </c>
     </row>
+    <row r="1276">
+      <c r="A1276" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1276" t="inlineStr">
+        <is>
+          <t>AD</t>
+        </is>
+      </c>
+      <c r="C1276" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D1276" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="1277">
+      <c r="A1277" t="inlineStr">
+        <is>
+          <t>NMB</t>
+        </is>
+      </c>
+      <c r="B1277" t="inlineStr">
+        <is>
+          <t>AD</t>
+        </is>
+      </c>
+      <c r="C1277" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D1277" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="1278">
+      <c r="A1278" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1278" t="inlineStr">
+        <is>
+          <t>AD</t>
+        </is>
+      </c>
+      <c r="C1278" t="inlineStr">
+        <is>
+          <t>overall</t>
+        </is>
+      </c>
+      <c r="D1278" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="1279">
+      <c r="A1279" t="inlineStr">
+        <is>
+          <t>NMB</t>
+        </is>
+      </c>
+      <c r="B1279" t="inlineStr">
+        <is>
+          <t>AD</t>
+        </is>
+      </c>
+      <c r="C1279" t="inlineStr">
+        <is>
+          <t>overall</t>
+        </is>
+      </c>
+      <c r="D1279" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="1280">
+      <c r="A1280" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1280" t="inlineStr">
+        <is>
+          <t>AD</t>
+        </is>
+      </c>
+      <c r="C1280" t="inlineStr">
+        <is>
+          <t>acts</t>
+        </is>
+      </c>
+      <c r="D1280" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="1281">
+      <c r="A1281" t="inlineStr">
+        <is>
+          <t>NMB</t>
+        </is>
+      </c>
+      <c r="B1281" t="inlineStr">
+        <is>
+          <t>AD</t>
+        </is>
+      </c>
+      <c r="C1281" t="inlineStr">
+        <is>
+          <t>acts</t>
+        </is>
+      </c>
+      <c r="D1281" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="1282">
+      <c r="A1282" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1282" t="inlineStr">
+        <is>
+          <t>AD</t>
+        </is>
+      </c>
+      <c r="C1282" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D1282" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="1283">
+      <c r="A1283" t="inlineStr">
+        <is>
+          <t>NMB</t>
+        </is>
+      </c>
+      <c r="B1283" t="inlineStr">
+        <is>
+          <t>AD</t>
+        </is>
+      </c>
+      <c r="C1283" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D1283" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="1284">
+      <c r="A1284" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1284" t="inlineStr">
+        <is>
+          <t>AD</t>
+        </is>
+      </c>
+      <c r="C1284" t="inlineStr">
+        <is>
+          <t>overall</t>
+        </is>
+      </c>
+      <c r="D1284" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="1285">
+      <c r="A1285" t="inlineStr">
+        <is>
+          <t>NMB</t>
+        </is>
+      </c>
+      <c r="B1285" t="inlineStr">
+        <is>
+          <t>AD</t>
+        </is>
+      </c>
+      <c r="C1285" t="inlineStr">
+        <is>
+          <t>overall</t>
+        </is>
+      </c>
+      <c r="D1285" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="1286">
+      <c r="A1286" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1286" t="inlineStr">
+        <is>
+          <t>AD</t>
+        </is>
+      </c>
+      <c r="C1286" t="inlineStr">
+        <is>
+          <t>acts</t>
+        </is>
+      </c>
+      <c r="D1286" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="1287">
+      <c r="A1287" t="inlineStr">
+        <is>
+          <t>NMB</t>
+        </is>
+      </c>
+      <c r="B1287" t="inlineStr">
+        <is>
+          <t>AD</t>
+        </is>
+      </c>
+      <c r="C1287" t="inlineStr">
+        <is>
+          <t>acts</t>
+        </is>
+      </c>
+      <c r="D1287" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="1288">
+      <c r="A1288" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1288" t="inlineStr">
+        <is>
+          <t>AD</t>
+        </is>
+      </c>
+      <c r="C1288" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D1288" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="1289">
+      <c r="A1289" t="inlineStr">
+        <is>
+          <t>NMB</t>
+        </is>
+      </c>
+      <c r="B1289" t="inlineStr">
+        <is>
+          <t>AD</t>
+        </is>
+      </c>
+      <c r="C1289" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D1289" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="1290">
+      <c r="A1290" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1290" t="inlineStr">
+        <is>
+          <t>AD</t>
+        </is>
+      </c>
+      <c r="C1290" t="inlineStr">
+        <is>
+          <t>overall</t>
+        </is>
+      </c>
+      <c r="D1290" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="1291">
+      <c r="A1291" t="inlineStr">
+        <is>
+          <t>NMB</t>
+        </is>
+      </c>
+      <c r="B1291" t="inlineStr">
+        <is>
+          <t>AD</t>
+        </is>
+      </c>
+      <c r="C1291" t="inlineStr">
+        <is>
+          <t>overall</t>
+        </is>
+      </c>
+      <c r="D1291" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="1292">
+      <c r="A1292" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1292" t="inlineStr">
+        <is>
+          <t>AD</t>
+        </is>
+      </c>
+      <c r="C1292" t="inlineStr">
+        <is>
+          <t>acts</t>
+        </is>
+      </c>
+      <c r="D1292" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="1293">
+      <c r="A1293" t="inlineStr">
+        <is>
+          <t>NMB</t>
+        </is>
+      </c>
+      <c r="B1293" t="inlineStr">
+        <is>
+          <t>AD</t>
+        </is>
+      </c>
+      <c r="C1293" t="inlineStr">
+        <is>
+          <t>acts</t>
+        </is>
+      </c>
+      <c r="D1293" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="1294">
+      <c r="A1294" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1294" t="inlineStr">
+        <is>
+          <t>AD</t>
+        </is>
+      </c>
+      <c r="C1294" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D1294" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="1295">
+      <c r="A1295" t="inlineStr">
+        <is>
+          <t>NMB</t>
+        </is>
+      </c>
+      <c r="B1295" t="inlineStr">
+        <is>
+          <t>AD</t>
+        </is>
+      </c>
+      <c r="C1295" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D1295" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="1296">
+      <c r="A1296" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1296" t="inlineStr">
+        <is>
+          <t>AD</t>
+        </is>
+      </c>
+      <c r="C1296" t="inlineStr">
+        <is>
+          <t>overall</t>
+        </is>
+      </c>
+      <c r="D1296" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="1297">
+      <c r="A1297" t="inlineStr">
+        <is>
+          <t>NMB</t>
+        </is>
+      </c>
+      <c r="B1297" t="inlineStr">
+        <is>
+          <t>AD</t>
+        </is>
+      </c>
+      <c r="C1297" t="inlineStr">
+        <is>
+          <t>overall</t>
+        </is>
+      </c>
+      <c r="D1297" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="1298">
+      <c r="A1298" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1298" t="inlineStr">
+        <is>
+          <t>AD</t>
+        </is>
+      </c>
+      <c r="C1298" t="inlineStr">
+        <is>
+          <t>acts</t>
+        </is>
+      </c>
+      <c r="D1298" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="1299">
+      <c r="A1299" t="inlineStr">
+        <is>
+          <t>NMB</t>
+        </is>
+      </c>
+      <c r="B1299" t="inlineStr">
+        <is>
+          <t>AD</t>
+        </is>
+      </c>
+      <c r="C1299" t="inlineStr">
+        <is>
+          <t>acts</t>
+        </is>
+      </c>
+      <c r="D1299" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="1300">
+      <c r="A1300" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1300" t="inlineStr">
+        <is>
+          <t>AD</t>
+        </is>
+      </c>
+      <c r="C1300" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D1300" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="1301">
+      <c r="A1301" t="inlineStr">
+        <is>
+          <t>NMB</t>
+        </is>
+      </c>
+      <c r="B1301" t="inlineStr">
+        <is>
+          <t>AD</t>
+        </is>
+      </c>
+      <c r="C1301" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D1301" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="1302">
+      <c r="A1302" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1302" t="inlineStr">
+        <is>
+          <t>AD</t>
+        </is>
+      </c>
+      <c r="C1302" t="inlineStr">
+        <is>
+          <t>overall</t>
+        </is>
+      </c>
+      <c r="D1302" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="1303">
+      <c r="A1303" t="inlineStr">
+        <is>
+          <t>NMB</t>
+        </is>
+      </c>
+      <c r="B1303" t="inlineStr">
+        <is>
+          <t>AD</t>
+        </is>
+      </c>
+      <c r="C1303" t="inlineStr">
+        <is>
+          <t>overall</t>
+        </is>
+      </c>
+      <c r="D1303" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="1304">
+      <c r="A1304" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1304" t="inlineStr">
+        <is>
+          <t>AD</t>
+        </is>
+      </c>
+      <c r="C1304" t="inlineStr">
+        <is>
+          <t>acts</t>
+        </is>
+      </c>
+      <c r="D1304" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="1305">
+      <c r="A1305" t="inlineStr">
+        <is>
+          <t>NMB</t>
+        </is>
+      </c>
+      <c r="B1305" t="inlineStr">
+        <is>
+          <t>AD</t>
+        </is>
+      </c>
+      <c r="C1305" t="inlineStr">
+        <is>
+          <t>acts</t>
+        </is>
+      </c>
+      <c r="D1305" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="1306">
+      <c r="A1306" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1306" t="inlineStr">
+        <is>
+          <t>position</t>
+        </is>
+      </c>
+      <c r="C1306" t="inlineStr">
+        <is>
+          <t>acts</t>
+        </is>
+      </c>
+      <c r="D1306" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1307">
+      <c r="A1307" t="inlineStr">
+        <is>
+          <t>NMB</t>
+        </is>
+      </c>
+      <c r="B1307" t="inlineStr">
+        <is>
+          <t>position</t>
+        </is>
+      </c>
+      <c r="C1307" t="inlineStr">
+        <is>
+          <t>acts</t>
+        </is>
+      </c>
+      <c r="D1307" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1308">
+      <c r="A1308" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1308" t="inlineStr">
+        <is>
+          <t>sensorMagneticField</t>
+        </is>
+      </c>
+      <c r="C1308" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D1308" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1309">
+      <c r="A1309" t="inlineStr">
+        <is>
+          <t>NMB</t>
+        </is>
+      </c>
+      <c r="B1309" t="inlineStr">
+        <is>
+          <t>sensorMagneticField</t>
+        </is>
+      </c>
+      <c r="C1309" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D1309" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1310">
+      <c r="A1310" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1310" t="inlineStr">
+        <is>
+          <t>sensorMagneticField</t>
+        </is>
+      </c>
+      <c r="C1310" t="inlineStr">
+        <is>
+          <t>overall</t>
+        </is>
+      </c>
+      <c r="D1310" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1311">
+      <c r="A1311" t="inlineStr">
+        <is>
+          <t>NMB</t>
+        </is>
+      </c>
+      <c r="B1311" t="inlineStr">
+        <is>
+          <t>sensorMagneticField</t>
+        </is>
+      </c>
+      <c r="C1311" t="inlineStr">
+        <is>
+          <t>overall</t>
+        </is>
+      </c>
+      <c r="D1311" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1312">
+      <c r="A1312" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1312" t="inlineStr">
+        <is>
+          <t>sensorMagneticField</t>
+        </is>
+      </c>
+      <c r="C1312" t="inlineStr">
+        <is>
+          <t>acts</t>
+        </is>
+      </c>
+      <c r="D1312" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1313">
+      <c r="A1313" t="inlineStr">
+        <is>
+          <t>NMB</t>
+        </is>
+      </c>
+      <c r="B1313" t="inlineStr">
+        <is>
+          <t>sensorMagneticField</t>
+        </is>
+      </c>
+      <c r="C1313" t="inlineStr">
+        <is>
+          <t>acts</t>
+        </is>
+      </c>
+      <c r="D1313" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1314">
+      <c r="A1314" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1314" t="inlineStr">
+        <is>
+          <t>jointAngle</t>
+        </is>
+      </c>
+      <c r="C1314" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D1314" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1315">
+      <c r="A1315" t="inlineStr">
+        <is>
+          <t>NMB</t>
+        </is>
+      </c>
+      <c r="B1315" t="inlineStr">
+        <is>
+          <t>jointAngle</t>
+        </is>
+      </c>
+      <c r="C1315" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D1315" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1316">
+      <c r="A1316" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1316" t="inlineStr">
+        <is>
+          <t>jointAngle</t>
+        </is>
+      </c>
+      <c r="C1316" t="inlineStr">
+        <is>
+          <t>overall</t>
+        </is>
+      </c>
+      <c r="D1316" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1317">
+      <c r="A1317" t="inlineStr">
+        <is>
+          <t>NMB</t>
+        </is>
+      </c>
+      <c r="B1317" t="inlineStr">
+        <is>
+          <t>jointAngle</t>
+        </is>
+      </c>
+      <c r="C1317" t="inlineStr">
+        <is>
+          <t>overall</t>
+        </is>
+      </c>
+      <c r="D1317" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1318">
+      <c r="A1318" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1318" t="inlineStr">
+        <is>
+          <t>jointAngle</t>
+        </is>
+      </c>
+      <c r="C1318" t="inlineStr">
+        <is>
+          <t>acts</t>
+        </is>
+      </c>
+      <c r="D1318" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1319">
+      <c r="A1319" t="inlineStr">
+        <is>
+          <t>NMB</t>
+        </is>
+      </c>
+      <c r="B1319" t="inlineStr">
+        <is>
+          <t>jointAngle</t>
+        </is>
+      </c>
+      <c r="C1319" t="inlineStr">
+        <is>
+          <t>acts</t>
+        </is>
+      </c>
+      <c r="D1319" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1320">
+      <c r="A1320" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1320" t="inlineStr">
+        <is>
+          <t>AD</t>
+        </is>
+      </c>
+      <c r="C1320" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D1320" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="1321">
+      <c r="A1321" t="inlineStr">
+        <is>
+          <t>NMB</t>
+        </is>
+      </c>
+      <c r="B1321" t="inlineStr">
+        <is>
+          <t>AD</t>
+        </is>
+      </c>
+      <c r="C1321" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D1321" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="1322">
+      <c r="A1322" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1322" t="inlineStr">
+        <is>
+          <t>AD</t>
+        </is>
+      </c>
+      <c r="C1322" t="inlineStr">
+        <is>
+          <t>overall</t>
+        </is>
+      </c>
+      <c r="D1322" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="1323">
+      <c r="A1323" t="inlineStr">
+        <is>
+          <t>NMB</t>
+        </is>
+      </c>
+      <c r="B1323" t="inlineStr">
+        <is>
+          <t>AD</t>
+        </is>
+      </c>
+      <c r="C1323" t="inlineStr">
+        <is>
+          <t>overall</t>
+        </is>
+      </c>
+      <c r="D1323" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="1324">
+      <c r="A1324" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1324" t="inlineStr">
+        <is>
+          <t>AD</t>
+        </is>
+      </c>
+      <c r="C1324" t="inlineStr">
+        <is>
+          <t>acts</t>
+        </is>
+      </c>
+      <c r="D1324" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="1325">
+      <c r="A1325" t="inlineStr">
+        <is>
+          <t>NMB</t>
+        </is>
+      </c>
+      <c r="B1325" t="inlineStr">
+        <is>
+          <t>AD</t>
+        </is>
+      </c>
+      <c r="C1325" t="inlineStr">
+        <is>
+          <t>acts</t>
+        </is>
+      </c>
+      <c r="D1325" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="1326">
+      <c r="A1326" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1326" t="inlineStr">
+        <is>
+          <t>position</t>
+        </is>
+      </c>
+      <c r="C1326" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D1326" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1327">
+      <c r="A1327" t="inlineStr">
+        <is>
+          <t>NMB</t>
+        </is>
+      </c>
+      <c r="B1327" t="inlineStr">
+        <is>
+          <t>position</t>
+        </is>
+      </c>
+      <c r="C1327" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D1327" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1328">
+      <c r="A1328" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1328" t="inlineStr">
+        <is>
+          <t>position</t>
+        </is>
+      </c>
+      <c r="C1328" t="inlineStr">
+        <is>
+          <t>overall</t>
+        </is>
+      </c>
+      <c r="D1328" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1329">
+      <c r="A1329" t="inlineStr">
+        <is>
+          <t>NMB</t>
+        </is>
+      </c>
+      <c r="B1329" t="inlineStr">
+        <is>
+          <t>position</t>
+        </is>
+      </c>
+      <c r="C1329" t="inlineStr">
+        <is>
+          <t>overall</t>
+        </is>
+      </c>
+      <c r="D1329" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1330">
+      <c r="A1330" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1330" t="inlineStr">
+        <is>
+          <t>position</t>
+        </is>
+      </c>
+      <c r="C1330" t="inlineStr">
+        <is>
+          <t>acts</t>
+        </is>
+      </c>
+      <c r="D1330" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1331">
+      <c r="A1331" t="inlineStr">
+        <is>
+          <t>NMB</t>
+        </is>
+      </c>
+      <c r="B1331" t="inlineStr">
+        <is>
+          <t>position</t>
+        </is>
+      </c>
+      <c r="C1331" t="inlineStr">
+        <is>
+          <t>acts</t>
+        </is>
+      </c>
+      <c r="D1331" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1332">
+      <c r="A1332" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1332" t="inlineStr">
+        <is>
+          <t>sensorMagneticField</t>
+        </is>
+      </c>
+      <c r="C1332" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D1332" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1333">
+      <c r="A1333" t="inlineStr">
+        <is>
+          <t>NMB</t>
+        </is>
+      </c>
+      <c r="B1333" t="inlineStr">
+        <is>
+          <t>sensorMagneticField</t>
+        </is>
+      </c>
+      <c r="C1333" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D1333" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1334">
+      <c r="A1334" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1334" t="inlineStr">
+        <is>
+          <t>sensorMagneticField</t>
+        </is>
+      </c>
+      <c r="C1334" t="inlineStr">
+        <is>
+          <t>overall</t>
+        </is>
+      </c>
+      <c r="D1334" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1335">
+      <c r="A1335" t="inlineStr">
+        <is>
+          <t>NMB</t>
+        </is>
+      </c>
+      <c r="B1335" t="inlineStr">
+        <is>
+          <t>sensorMagneticField</t>
+        </is>
+      </c>
+      <c r="C1335" t="inlineStr">
+        <is>
+          <t>overall</t>
+        </is>
+      </c>
+      <c r="D1335" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1336">
+      <c r="A1336" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1336" t="inlineStr">
+        <is>
+          <t>sensorMagneticField</t>
+        </is>
+      </c>
+      <c r="C1336" t="inlineStr">
+        <is>
+          <t>acts</t>
+        </is>
+      </c>
+      <c r="D1336" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1337">
+      <c r="A1337" t="inlineStr">
+        <is>
+          <t>NMB</t>
+        </is>
+      </c>
+      <c r="B1337" t="inlineStr">
+        <is>
+          <t>sensorMagneticField</t>
+        </is>
+      </c>
+      <c r="C1337" t="inlineStr">
+        <is>
+          <t>acts</t>
+        </is>
+      </c>
+      <c r="D1337" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1338">
+      <c r="A1338" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1338" t="inlineStr">
+        <is>
+          <t>jointAngle</t>
+        </is>
+      </c>
+      <c r="C1338" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D1338" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1339">
+      <c r="A1339" t="inlineStr">
+        <is>
+          <t>NMB</t>
+        </is>
+      </c>
+      <c r="B1339" t="inlineStr">
+        <is>
+          <t>jointAngle</t>
+        </is>
+      </c>
+      <c r="C1339" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D1339" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1340">
+      <c r="A1340" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1340" t="inlineStr">
+        <is>
+          <t>jointAngle</t>
+        </is>
+      </c>
+      <c r="C1340" t="inlineStr">
+        <is>
+          <t>overall</t>
+        </is>
+      </c>
+      <c r="D1340" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1341">
+      <c r="A1341" t="inlineStr">
+        <is>
+          <t>NMB</t>
+        </is>
+      </c>
+      <c r="B1341" t="inlineStr">
+        <is>
+          <t>jointAngle</t>
+        </is>
+      </c>
+      <c r="C1341" t="inlineStr">
+        <is>
+          <t>overall</t>
+        </is>
+      </c>
+      <c r="D1341" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1342">
+      <c r="A1342" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1342" t="inlineStr">
+        <is>
+          <t>jointAngle</t>
+        </is>
+      </c>
+      <c r="C1342" t="inlineStr">
+        <is>
+          <t>acts</t>
+        </is>
+      </c>
+      <c r="D1342" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1343">
+      <c r="A1343" t="inlineStr">
+        <is>
+          <t>NMB</t>
+        </is>
+      </c>
+      <c r="B1343" t="inlineStr">
+        <is>
+          <t>jointAngle</t>
+        </is>
+      </c>
+      <c r="C1343" t="inlineStr">
+        <is>
+          <t>acts</t>
+        </is>
+      </c>
+      <c r="D1343" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1344">
+      <c r="A1344" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1344" t="inlineStr">
+        <is>
+          <t>AD</t>
+        </is>
+      </c>
+      <c r="C1344" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D1344" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="1345">
+      <c r="A1345" t="inlineStr">
+        <is>
+          <t>NMB</t>
+        </is>
+      </c>
+      <c r="B1345" t="inlineStr">
+        <is>
+          <t>AD</t>
+        </is>
+      </c>
+      <c r="C1345" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D1345" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="1346">
+      <c r="A1346" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1346" t="inlineStr">
+        <is>
+          <t>AD</t>
+        </is>
+      </c>
+      <c r="C1346" t="inlineStr">
+        <is>
+          <t>overall</t>
+        </is>
+      </c>
+      <c r="D1346" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="1347">
+      <c r="A1347" t="inlineStr">
+        <is>
+          <t>NMB</t>
+        </is>
+      </c>
+      <c r="B1347" t="inlineStr">
+        <is>
+          <t>AD</t>
+        </is>
+      </c>
+      <c r="C1347" t="inlineStr">
+        <is>
+          <t>overall</t>
+        </is>
+      </c>
+      <c r="D1347" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="1348">
+      <c r="A1348" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1348" t="inlineStr">
+        <is>
+          <t>AD</t>
+        </is>
+      </c>
+      <c r="C1348" t="inlineStr">
+        <is>
+          <t>acts</t>
+        </is>
+      </c>
+      <c r="D1348" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="1349">
+      <c r="A1349" t="inlineStr">
+        <is>
+          <t>NMB</t>
+        </is>
+      </c>
+      <c r="B1349" t="inlineStr">
+        <is>
+          <t>AD</t>
+        </is>
+      </c>
+      <c r="C1349" t="inlineStr">
+        <is>
+          <t>acts</t>
+        </is>
+      </c>
+      <c r="D1349" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="1350">
+      <c r="A1350" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1350" t="inlineStr">
+        <is>
+          <t>position</t>
+        </is>
+      </c>
+      <c r="C1350" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D1350" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1351">
+      <c r="A1351" t="inlineStr">
+        <is>
+          <t>NMB</t>
+        </is>
+      </c>
+      <c r="B1351" t="inlineStr">
+        <is>
+          <t>position</t>
+        </is>
+      </c>
+      <c r="C1351" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D1351" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1352">
+      <c r="A1352" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1352" t="inlineStr">
+        <is>
+          <t>position</t>
+        </is>
+      </c>
+      <c r="C1352" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D1352" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1353">
+      <c r="A1353" t="inlineStr">
+        <is>
+          <t>NMB</t>
+        </is>
+      </c>
+      <c r="B1353" t="inlineStr">
+        <is>
+          <t>position</t>
+        </is>
+      </c>
+      <c r="C1353" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D1353" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1354">
+      <c r="A1354" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1354" t="inlineStr">
+        <is>
+          <t>position</t>
+        </is>
+      </c>
+      <c r="C1354" t="inlineStr">
+        <is>
+          <t>overall</t>
+        </is>
+      </c>
+      <c r="D1354" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1355">
+      <c r="A1355" t="inlineStr">
+        <is>
+          <t>NMB</t>
+        </is>
+      </c>
+      <c r="B1355" t="inlineStr">
+        <is>
+          <t>position</t>
+        </is>
+      </c>
+      <c r="C1355" t="inlineStr">
+        <is>
+          <t>overall</t>
+        </is>
+      </c>
+      <c r="D1355" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1356">
+      <c r="A1356" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1356" t="inlineStr">
+        <is>
+          <t>position</t>
+        </is>
+      </c>
+      <c r="C1356" t="inlineStr">
+        <is>
+          <t>acts</t>
+        </is>
+      </c>
+      <c r="D1356" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1357">
+      <c r="A1357" t="inlineStr">
+        <is>
+          <t>NMB</t>
+        </is>
+      </c>
+      <c r="B1357" t="inlineStr">
+        <is>
+          <t>position</t>
+        </is>
+      </c>
+      <c r="C1357" t="inlineStr">
+        <is>
+          <t>acts</t>
+        </is>
+      </c>
+      <c r="D1357" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1358">
+      <c r="A1358" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1358" t="inlineStr">
+        <is>
+          <t>sensorMagneticField</t>
+        </is>
+      </c>
+      <c r="C1358" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D1358" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1359">
+      <c r="A1359" t="inlineStr">
+        <is>
+          <t>NMB</t>
+        </is>
+      </c>
+      <c r="B1359" t="inlineStr">
+        <is>
+          <t>sensorMagneticField</t>
+        </is>
+      </c>
+      <c r="C1359" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D1359" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1360">
+      <c r="A1360" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1360" t="inlineStr">
+        <is>
+          <t>sensorMagneticField</t>
+        </is>
+      </c>
+      <c r="C1360" t="inlineStr">
+        <is>
+          <t>overall</t>
+        </is>
+      </c>
+      <c r="D1360" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1361">
+      <c r="A1361" t="inlineStr">
+        <is>
+          <t>NMB</t>
+        </is>
+      </c>
+      <c r="B1361" t="inlineStr">
+        <is>
+          <t>sensorMagneticField</t>
+        </is>
+      </c>
+      <c r="C1361" t="inlineStr">
+        <is>
+          <t>overall</t>
+        </is>
+      </c>
+      <c r="D1361" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1362">
+      <c r="A1362" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1362" t="inlineStr">
+        <is>
+          <t>sensorMagneticField</t>
+        </is>
+      </c>
+      <c r="C1362" t="inlineStr">
+        <is>
+          <t>acts</t>
+        </is>
+      </c>
+      <c r="D1362" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1363">
+      <c r="A1363" t="inlineStr">
+        <is>
+          <t>NMB</t>
+        </is>
+      </c>
+      <c r="B1363" t="inlineStr">
+        <is>
+          <t>sensorMagneticField</t>
+        </is>
+      </c>
+      <c r="C1363" t="inlineStr">
+        <is>
+          <t>acts</t>
+        </is>
+      </c>
+      <c r="D1363" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1364">
+      <c r="A1364" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1364" t="inlineStr">
+        <is>
+          <t>jointAngle</t>
+        </is>
+      </c>
+      <c r="C1364" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D1364" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1365">
+      <c r="A1365" t="inlineStr">
+        <is>
+          <t>NMB</t>
+        </is>
+      </c>
+      <c r="B1365" t="inlineStr">
+        <is>
+          <t>jointAngle</t>
+        </is>
+      </c>
+      <c r="C1365" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D1365" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1366">
+      <c r="A1366" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1366" t="inlineStr">
+        <is>
+          <t>jointAngle</t>
+        </is>
+      </c>
+      <c r="C1366" t="inlineStr">
+        <is>
+          <t>overall</t>
+        </is>
+      </c>
+      <c r="D1366" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1367">
+      <c r="A1367" t="inlineStr">
+        <is>
+          <t>NMB</t>
+        </is>
+      </c>
+      <c r="B1367" t="inlineStr">
+        <is>
+          <t>jointAngle</t>
+        </is>
+      </c>
+      <c r="C1367" t="inlineStr">
+        <is>
+          <t>overall</t>
+        </is>
+      </c>
+      <c r="D1367" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1368">
+      <c r="A1368" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1368" t="inlineStr">
+        <is>
+          <t>jointAngle</t>
+        </is>
+      </c>
+      <c r="C1368" t="inlineStr">
+        <is>
+          <t>acts</t>
+        </is>
+      </c>
+      <c r="D1368" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1369">
+      <c r="A1369" t="inlineStr">
+        <is>
+          <t>NMB</t>
+        </is>
+      </c>
+      <c r="B1369" t="inlineStr">
+        <is>
+          <t>jointAngle</t>
+        </is>
+      </c>
+      <c r="C1369" t="inlineStr">
+        <is>
+          <t>acts</t>
+        </is>
+      </c>
+      <c r="D1369" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1370">
+      <c r="A1370" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1370" t="inlineStr">
+        <is>
+          <t>AD</t>
+        </is>
+      </c>
+      <c r="C1370" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D1370" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="1371">
+      <c r="A1371" t="inlineStr">
+        <is>
+          <t>NMB</t>
+        </is>
+      </c>
+      <c r="B1371" t="inlineStr">
+        <is>
+          <t>AD</t>
+        </is>
+      </c>
+      <c r="C1371" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D1371" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="1372">
+      <c r="A1372" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1372" t="inlineStr">
+        <is>
+          <t>AD</t>
+        </is>
+      </c>
+      <c r="C1372" t="inlineStr">
+        <is>
+          <t>overall</t>
+        </is>
+      </c>
+      <c r="D1372" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="1373">
+      <c r="A1373" t="inlineStr">
+        <is>
+          <t>NMB</t>
+        </is>
+      </c>
+      <c r="B1373" t="inlineStr">
+        <is>
+          <t>AD</t>
+        </is>
+      </c>
+      <c r="C1373" t="inlineStr">
+        <is>
+          <t>overall</t>
+        </is>
+      </c>
+      <c r="D1373" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="1374">
+      <c r="A1374" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1374" t="inlineStr">
+        <is>
+          <t>AD</t>
+        </is>
+      </c>
+      <c r="C1374" t="inlineStr">
+        <is>
+          <t>acts</t>
+        </is>
+      </c>
+      <c r="D1374" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="1375">
+      <c r="A1375" t="inlineStr">
+        <is>
+          <t>NMB</t>
+        </is>
+      </c>
+      <c r="B1375" t="inlineStr">
+        <is>
+          <t>AD</t>
+        </is>
+      </c>
+      <c r="C1375" t="inlineStr">
+        <is>
+          <t>acts</t>
+        </is>
+      </c>
+      <c r="D1375" t="n">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>

<commit_message>
Added project timeline/Gantt chart, further improvements to be made, setup LaTeX inner-directory, wrote part 1 of LaTeX final report, conducted several more model predictions sets and modified 'source' files to work with them, added a batch script to assess new NSAA subjects, and added several top-level README's to the repo.
</commit_message>
<xml_diff>
--- a/documentation/model_shapes.xlsx
+++ b/documentation/model_shapes.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D1375"/>
+  <dimension ref="A1:D1402"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -27868,6 +27868,546 @@
         <v>10</v>
       </c>
     </row>
+    <row r="1376">
+      <c r="A1376" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1376" t="inlineStr">
+        <is>
+          <t>position</t>
+        </is>
+      </c>
+      <c r="C1376" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D1376" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1377">
+      <c r="A1377" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1377" t="inlineStr">
+        <is>
+          <t>position</t>
+        </is>
+      </c>
+      <c r="C1377" t="inlineStr">
+        <is>
+          <t>overall</t>
+        </is>
+      </c>
+      <c r="D1377" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1378">
+      <c r="A1378" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1378" t="inlineStr">
+        <is>
+          <t>position</t>
+        </is>
+      </c>
+      <c r="C1378" t="inlineStr">
+        <is>
+          <t>acts</t>
+        </is>
+      </c>
+      <c r="D1378" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1379">
+      <c r="A1379" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1379" t="inlineStr">
+        <is>
+          <t>sensorMagneticField</t>
+        </is>
+      </c>
+      <c r="C1379" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D1379" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1380">
+      <c r="A1380" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1380" t="inlineStr">
+        <is>
+          <t>sensorMagneticField</t>
+        </is>
+      </c>
+      <c r="C1380" t="inlineStr">
+        <is>
+          <t>overall</t>
+        </is>
+      </c>
+      <c r="D1380" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1381">
+      <c r="A1381" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1381" t="inlineStr">
+        <is>
+          <t>sensorMagneticField</t>
+        </is>
+      </c>
+      <c r="C1381" t="inlineStr">
+        <is>
+          <t>acts</t>
+        </is>
+      </c>
+      <c r="D1381" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1382">
+      <c r="A1382" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1382" t="inlineStr">
+        <is>
+          <t>jointAngle</t>
+        </is>
+      </c>
+      <c r="C1382" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D1382" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1383">
+      <c r="A1383" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1383" t="inlineStr">
+        <is>
+          <t>jointAngle</t>
+        </is>
+      </c>
+      <c r="C1383" t="inlineStr">
+        <is>
+          <t>overall</t>
+        </is>
+      </c>
+      <c r="D1383" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1384">
+      <c r="A1384" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1384" t="inlineStr">
+        <is>
+          <t>jointAngle</t>
+        </is>
+      </c>
+      <c r="C1384" t="inlineStr">
+        <is>
+          <t>acts</t>
+        </is>
+      </c>
+      <c r="D1384" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1385">
+      <c r="A1385" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1385" t="inlineStr">
+        <is>
+          <t>AD</t>
+        </is>
+      </c>
+      <c r="C1385" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D1385" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="1386">
+      <c r="A1386" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1386" t="inlineStr">
+        <is>
+          <t>AD</t>
+        </is>
+      </c>
+      <c r="C1386" t="inlineStr">
+        <is>
+          <t>overall</t>
+        </is>
+      </c>
+      <c r="D1386" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="1387">
+      <c r="A1387" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B1387" t="inlineStr">
+        <is>
+          <t>AD</t>
+        </is>
+      </c>
+      <c r="C1387" t="inlineStr">
+        <is>
+          <t>acts</t>
+        </is>
+      </c>
+      <c r="D1387" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="1388">
+      <c r="A1388" t="inlineStr">
+        <is>
+          <t>NMB</t>
+        </is>
+      </c>
+      <c r="B1388" t="inlineStr">
+        <is>
+          <t>position</t>
+        </is>
+      </c>
+      <c r="C1388" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D1388" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1389">
+      <c r="A1389" t="inlineStr">
+        <is>
+          <t>NMB</t>
+        </is>
+      </c>
+      <c r="B1389" t="inlineStr">
+        <is>
+          <t>position</t>
+        </is>
+      </c>
+      <c r="C1389" t="inlineStr">
+        <is>
+          <t>overall</t>
+        </is>
+      </c>
+      <c r="D1389" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1390">
+      <c r="A1390" t="inlineStr">
+        <is>
+          <t>NMB</t>
+        </is>
+      </c>
+      <c r="B1390" t="inlineStr">
+        <is>
+          <t>position</t>
+        </is>
+      </c>
+      <c r="C1390" t="inlineStr">
+        <is>
+          <t>acts</t>
+        </is>
+      </c>
+      <c r="D1390" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1391">
+      <c r="A1391" t="inlineStr">
+        <is>
+          <t>NMB</t>
+        </is>
+      </c>
+      <c r="B1391" t="inlineStr">
+        <is>
+          <t>sensorMagneticField</t>
+        </is>
+      </c>
+      <c r="C1391" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D1391" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1392">
+      <c r="A1392" t="inlineStr">
+        <is>
+          <t>NMB</t>
+        </is>
+      </c>
+      <c r="B1392" t="inlineStr">
+        <is>
+          <t>sensorMagneticField</t>
+        </is>
+      </c>
+      <c r="C1392" t="inlineStr">
+        <is>
+          <t>overall</t>
+        </is>
+      </c>
+      <c r="D1392" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1393">
+      <c r="A1393" t="inlineStr">
+        <is>
+          <t>NMB</t>
+        </is>
+      </c>
+      <c r="B1393" t="inlineStr">
+        <is>
+          <t>sensorMagneticField</t>
+        </is>
+      </c>
+      <c r="C1393" t="inlineStr">
+        <is>
+          <t>acts</t>
+        </is>
+      </c>
+      <c r="D1393" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1394">
+      <c r="A1394" t="inlineStr">
+        <is>
+          <t>NMB</t>
+        </is>
+      </c>
+      <c r="B1394" t="inlineStr">
+        <is>
+          <t>jointAngle</t>
+        </is>
+      </c>
+      <c r="C1394" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D1394" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1395">
+      <c r="A1395" t="inlineStr">
+        <is>
+          <t>NMB</t>
+        </is>
+      </c>
+      <c r="B1395" t="inlineStr">
+        <is>
+          <t>jointAngle</t>
+        </is>
+      </c>
+      <c r="C1395" t="inlineStr">
+        <is>
+          <t>overall</t>
+        </is>
+      </c>
+      <c r="D1395" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1396">
+      <c r="A1396" t="inlineStr">
+        <is>
+          <t>NMB</t>
+        </is>
+      </c>
+      <c r="B1396" t="inlineStr">
+        <is>
+          <t>jointAngle</t>
+        </is>
+      </c>
+      <c r="C1396" t="inlineStr">
+        <is>
+          <t>acts</t>
+        </is>
+      </c>
+      <c r="D1396" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1397">
+      <c r="A1397" t="inlineStr">
+        <is>
+          <t>NMB</t>
+        </is>
+      </c>
+      <c r="B1397" t="inlineStr">
+        <is>
+          <t>AD</t>
+        </is>
+      </c>
+      <c r="C1397" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D1397" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="1398">
+      <c r="A1398" t="inlineStr">
+        <is>
+          <t>NMB</t>
+        </is>
+      </c>
+      <c r="B1398" t="inlineStr">
+        <is>
+          <t>AD</t>
+        </is>
+      </c>
+      <c r="C1398" t="inlineStr">
+        <is>
+          <t>overall</t>
+        </is>
+      </c>
+      <c r="D1398" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="1399">
+      <c r="A1399" t="inlineStr">
+        <is>
+          <t>NMB</t>
+        </is>
+      </c>
+      <c r="B1399" t="inlineStr">
+        <is>
+          <t>AD</t>
+        </is>
+      </c>
+      <c r="C1399" t="inlineStr">
+        <is>
+          <t>acts</t>
+        </is>
+      </c>
+      <c r="D1399" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="1400">
+      <c r="A1400" t="inlineStr">
+        <is>
+          <t>NMB</t>
+        </is>
+      </c>
+      <c r="B1400" t="inlineStr">
+        <is>
+          <t>AD</t>
+        </is>
+      </c>
+      <c r="C1400" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D1400" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="1401">
+      <c r="A1401" t="inlineStr">
+        <is>
+          <t>NMB</t>
+        </is>
+      </c>
+      <c r="B1401" t="inlineStr">
+        <is>
+          <t>AD</t>
+        </is>
+      </c>
+      <c r="C1401" t="inlineStr">
+        <is>
+          <t>overall</t>
+        </is>
+      </c>
+      <c r="D1401" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="1402">
+      <c r="A1402" t="inlineStr">
+        <is>
+          <t>NMB</t>
+        </is>
+      </c>
+      <c r="B1402" t="inlineStr">
+        <is>
+          <t>AD</t>
+        </is>
+      </c>
+      <c r="C1402" t="inlineStr">
+        <is>
+          <t>acts</t>
+        </is>
+      </c>
+      <c r="D1402" t="n">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>